<commit_message>
This is still from MacMini in future to be reversed.
</commit_message>
<xml_diff>
--- a/tables/slr_logbook.xlsx
+++ b/tables/slr_logbook.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Library/CloudStorage/OneDrive-VlerickBusinessSchool/_2023.12/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Projects/literature/phd_kul/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{591A33DE-9996-A442-94BE-D808EC8FEB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5E7FB6-D14B-6A46-899D-B2C24B2BF2CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36860" yWindow="4740" windowWidth="36160" windowHeight="36180" activeTab="2" xr2:uid="{AC0C9749-44FB-E246-A4D0-62D1F20133DE}"/>
+    <workbookView xWindow="37640" yWindow="1620" windowWidth="36160" windowHeight="36180" activeTab="2" xr2:uid="{AC0C9749-44FB-E246-A4D0-62D1F20133DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
     <sheet name="Pivot" sheetId="3" r:id="rId2"/>
-    <sheet name="2021" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="2021" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="16" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="195">
   <si>
     <t>Date</t>
   </si>
@@ -575,6 +576,108 @@
   <si>
     <t>"business process management" and "risk management" and "non financial information"</t>
   </si>
+  <si>
+    <t>Platform</t>
+  </si>
+  <si>
+    <t>Web of Science</t>
+  </si>
+  <si>
+    <t>ScienceDirect</t>
+  </si>
+  <si>
+    <t>SSRN</t>
+  </si>
+  <si>
+    <t>arXiv</t>
+  </si>
+  <si>
+    <t>DBLP</t>
+  </si>
+  <si>
+    <t>Zenodo</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Citation index</t>
+  </si>
+  <si>
+    <t>Academic literature platform</t>
+  </si>
+  <si>
+    <t>Preprints</t>
+  </si>
+  <si>
+    <t>Bibliography database</t>
+  </si>
+  <si>
+    <t>Dataset repository</t>
+  </si>
+  <si>
+    <t>Knowledge base</t>
+  </si>
+  <si>
+    <t>Focus</t>
+  </si>
+  <si>
+    <t>Wide range of disciplines (including hard sciences, social sciences, and the humanities)</t>
+  </si>
+  <si>
+    <t>Science, technology, medicine, and social science</t>
+  </si>
+  <si>
+    <t>Social sciences, economics, and business</t>
+  </si>
+  <si>
+    <t>Hard sciences and quantitative sciences</t>
+  </si>
+  <si>
+    <t>Computer science</t>
+  </si>
+  <si>
+    <t>Data from various disciplines</t>
+  </si>
+  <si>
+    <t>Academic publications and research outputs</t>
+  </si>
+  <si>
+    <t>Coverage</t>
+  </si>
+  <si>
+    <t>Over 18,000 academic journals, books, patents, and other scholarly publications</t>
+  </si>
+  <si>
+    <t>Over 3,500 peer-reviewed journals</t>
+  </si>
+  <si>
+    <t>Early-stage social science, economics, and business research papers</t>
+  </si>
+  <si>
+    <t>Early-stage research papers in a wide range of disciplines</t>
+  </si>
+  <si>
+    <t>Scholarly publications in computer science</t>
+  </si>
+  <si>
+    <t>Data from research projects, surveys, and other data collection efforts</t>
+  </si>
+  <si>
+    <t>Academic publications and research outputs from universities, research institutions, and scholarly societies</t>
+  </si>
+  <si>
+    <t>Access</t>
+  </si>
+  <si>
+    <t>Subscription-based</t>
+  </si>
+  <si>
+    <t>Subscription-based and open access</t>
+  </si>
+  <si>
+    <t>Open access</t>
+  </si>
 </sst>
 </file>
 
@@ -582,9 +685,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="169" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -646,20 +749,60 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4472C4"/>
+        <bgColor rgb="FF4472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FFD9E1F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -669,7 +812,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -686,7 +829,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -694,22 +837,270 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="23">
     <dxf>
-      <numFmt numFmtId="169" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4472C4"/>
+          <bgColor rgb="FF4472C4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
     </dxf>
     <dxf>
       <alignment horizontal="right"/>
@@ -718,46 +1109,7 @@
       <alignment horizontal="right"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -779,6 +1131,12 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1590,7 +1948,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7BE126E1-EB43-D243-9887-A5AB93F74BC1}" name="PivotTable2" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Total" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7BE126E1-EB43-D243-9887-A5AB93F74BC1}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Total" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:H11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -1682,20 +2040,20 @@
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of Quantity" fld="7" baseField="0" baseItem="0" numFmtId="169"/>
+    <dataField name="Sum of Quantity" fld="7" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="11">
+    <format dxfId="12">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -1712,27 +2070,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FFF0228E-16A0-0745-BA5A-B606859071BD}" name="Table1" displayName="Table1" ref="A7:I73" totalsRowShown="0" headerRowDxfId="15" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FFF0228E-16A0-0745-BA5A-B606859071BD}" name="Table1" displayName="Table1" ref="A7:I73" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A7:I73" xr:uid="{FFF0228E-16A0-0745-BA5A-B606859071BD}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{ABE8919E-31E3-3C4D-BE26-E0B097FD8BAF}" name="Record" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{DCEAF83F-13E5-F04F-959B-309C1258F8D6}" name="Date" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{7D890402-E0DD-7941-A452-A014F2CD93DD}" name="Steps taken" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{32C6624E-63B0-B64B-AB39-6467D72B490D}" name="Database" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{8C094E55-9E0E-FC42-9895-83D32CEF90A9}" name="QueryNr" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{2FFD36BC-A2D2-A848-868B-212869119555}" name="QuerySubNr" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{ABE8919E-31E3-3C4D-BE26-E0B097FD8BAF}" name="Record" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{DCEAF83F-13E5-F04F-959B-309C1258F8D6}" name="Date" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{7D890402-E0DD-7941-A452-A014F2CD93DD}" name="Steps taken" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{32C6624E-63B0-B64B-AB39-6467D72B490D}" name="Database" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{8C094E55-9E0E-FC42-9895-83D32CEF90A9}" name="QueryNr" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{2FFD36BC-A2D2-A848-868B-212869119555}" name="QuerySubNr" dataDxfId="15"/>
     <tableColumn id="7" xr3:uid="{762D1B3E-C5F1-6D43-B97F-55EAA8FDB56C}" name="QueryString"/>
-    <tableColumn id="8" xr3:uid="{0E1EDC8C-20E2-CF43-9DE7-56E7C0BF256D}" name="Quantity" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{92D1697A-99F2-814E-A00C-ED758147A27A}" name="Notes / Comments" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{0E1EDC8C-20E2-CF43-9DE7-56E7C0BF256D}" name="Quantity" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{92D1697A-99F2-814E-A00C-ED758147A27A}" name="Notes / Comments" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A20822EB-39FA-6648-9837-2FAF2BBFC395}" name="Databases" displayName="Databases" ref="B2:I6" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="8">
+  <autoFilter ref="B2:I6" xr:uid="{A20822EB-39FA-6648-9837-2FAF2BBFC395}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{F4EF182A-30AC-754D-86FF-2E2ADCC705E9}" name="Platform"/>
+    <tableColumn id="2" xr3:uid="{56E9FBF2-2994-2748-B295-3DB88B2EDDD5}" name="Web of Science"/>
+    <tableColumn id="3" xr3:uid="{B0EF25B1-0375-C640-88C9-873752774E62}" name="ScienceDirect"/>
+    <tableColumn id="4" xr3:uid="{C76BBAAB-83F0-214C-9B08-4A1790A46529}" name="SSRN"/>
+    <tableColumn id="5" xr3:uid="{97018384-0991-9346-A86B-ECB7C17EF056}" name="arXiv"/>
+    <tableColumn id="6" xr3:uid="{47735B29-3713-604E-9ED9-F319585CB371}" name="DBLP"/>
+    <tableColumn id="7" xr3:uid="{0CAE628A-3842-C748-82DF-321D3A36E786}" name="Zenodo"/>
+    <tableColumn id="8" xr3:uid="{AAA42901-B756-6C47-93E9-9689444E6690}" name="OpenAlex"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{85AFCCCA-7255-F341-BACF-D289839D2415}" name="Database2" displayName="Database2" ref="B12:F19" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" tableBorderDxfId="7">
+  <autoFilter ref="B12:F19" xr:uid="{85AFCCCA-7255-F341-BACF-D289839D2415}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{7C68FF17-2976-BA4E-8999-5A67F8E9B01F}" name="Platform" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{7B36FC73-8715-2F4D-9E5C-5BE540BD7F64}" name="Type" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{2DD0E2CD-5A22-1C40-93AF-E88E2332E5A4}" name="Focus" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{24AAB514-0DA4-6D41-B622-DFFD00A34E8D}" name="Coverage" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{011D8E6E-C900-7648-8085-2B8D2880B641}" name="Access" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1770,7 +2159,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1876,7 +2265,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2018,7 +2407,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4173,7 +4562,7 @@
   <dimension ref="A3:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4409,10 +4798,301 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6764B6A2-AEB7-C544-9994-5A15BB9C9B07}">
+  <dimension ref="B2:I19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" customWidth="1"/>
+    <col min="9" max="9" width="11.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B2" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B3" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>194</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0824C28-D54F-324C-8E0D-94412A570CBC}">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update github repository with current version of local files.
</commit_message>
<xml_diff>
--- a/tables/slr_logbook.xlsx
+++ b/tables/slr_logbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Projects/literature/phd_kul/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5E7FB6-D14B-6A46-899D-B2C24B2BF2CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84211482-AE79-EA49-9694-7D54EA3BC3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37640" yWindow="1620" windowWidth="36160" windowHeight="36180" activeTab="2" xr2:uid="{AC0C9749-44FB-E246-A4D0-62D1F20133DE}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="208">
   <si>
     <t>Date</t>
   </si>
@@ -678,6 +678,45 @@
   <si>
     <t>Open access</t>
   </si>
+  <si>
+    <t>Run#</t>
+  </si>
+  <si>
+    <t>Query#</t>
+  </si>
+  <si>
+    <t>11/24/2023</t>
+  </si>
+  <si>
+    <t>Q01</t>
+  </si>
+  <si>
+    <t>Q02</t>
+  </si>
+  <si>
+    <t>Q03</t>
+  </si>
+  <si>
+    <t>Q04</t>
+  </si>
+  <si>
+    <t>Q05</t>
+  </si>
+  <si>
+    <t>Q06</t>
+  </si>
+  <si>
+    <t>dblp</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
 </sst>
 </file>
 
@@ -687,7 +726,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -762,6 +801,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -812,7 +859,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -856,13 +903,243 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="34">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4472C4"/>
+          <bgColor rgb="FF4472C4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2043,17 +2320,17 @@
     <dataField name="Sum of Quantity" fld="7" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="12">
+    <format dxfId="23">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="11">
+    <format dxfId="22">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -2070,25 +2347,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FFF0228E-16A0-0745-BA5A-B606859071BD}" name="Table1" displayName="Table1" ref="A7:I73" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FFF0228E-16A0-0745-BA5A-B606859071BD}" name="Table1" displayName="Table1" ref="A7:I73" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A7:I73" xr:uid="{FFF0228E-16A0-0745-BA5A-B606859071BD}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{ABE8919E-31E3-3C4D-BE26-E0B097FD8BAF}" name="Record" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{DCEAF83F-13E5-F04F-959B-309C1258F8D6}" name="Date" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{7D890402-E0DD-7941-A452-A014F2CD93DD}" name="Steps taken" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{32C6624E-63B0-B64B-AB39-6467D72B490D}" name="Database" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{8C094E55-9E0E-FC42-9895-83D32CEF90A9}" name="QueryNr" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{2FFD36BC-A2D2-A848-868B-212869119555}" name="QuerySubNr" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{ABE8919E-31E3-3C4D-BE26-E0B097FD8BAF}" name="Record" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{DCEAF83F-13E5-F04F-959B-309C1258F8D6}" name="Date" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{7D890402-E0DD-7941-A452-A014F2CD93DD}" name="Steps taken" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{32C6624E-63B0-B64B-AB39-6467D72B490D}" name="Database" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{8C094E55-9E0E-FC42-9895-83D32CEF90A9}" name="QueryNr" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{2FFD36BC-A2D2-A848-868B-212869119555}" name="QuerySubNr" dataDxfId="26"/>
     <tableColumn id="7" xr3:uid="{762D1B3E-C5F1-6D43-B97F-55EAA8FDB56C}" name="QueryString"/>
-    <tableColumn id="8" xr3:uid="{0E1EDC8C-20E2-CF43-9DE7-56E7C0BF256D}" name="Quantity" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{92D1697A-99F2-814E-A00C-ED758147A27A}" name="Notes / Comments" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{0E1EDC8C-20E2-CF43-9DE7-56E7C0BF256D}" name="Quantity" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{92D1697A-99F2-814E-A00C-ED758147A27A}" name="Notes / Comments" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A20822EB-39FA-6648-9837-2FAF2BBFC395}" name="Databases" displayName="Databases" ref="B2:I6" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A20822EB-39FA-6648-9837-2FAF2BBFC395}" name="Databases" displayName="Databases" ref="B2:I6" totalsRowShown="0" headerRowDxfId="20" tableBorderDxfId="19">
   <autoFilter ref="B2:I6" xr:uid="{A20822EB-39FA-6648-9837-2FAF2BBFC395}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F4EF182A-30AC-754D-86FF-2E2ADCC705E9}" name="Platform"/>
@@ -2105,14 +2382,32 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{85AFCCCA-7255-F341-BACF-D289839D2415}" name="Database2" displayName="Database2" ref="B12:F19" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{85AFCCCA-7255-F341-BACF-D289839D2415}" name="Database2" displayName="Database2" ref="B12:F19" totalsRowShown="0" headerRowDxfId="11" dataDxfId="12" tableBorderDxfId="18">
   <autoFilter ref="B12:F19" xr:uid="{85AFCCCA-7255-F341-BACF-D289839D2415}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7C68FF17-2976-BA4E-8999-5A67F8E9B01F}" name="Platform" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{7B36FC73-8715-2F4D-9E5C-5BE540BD7F64}" name="Type" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{2DD0E2CD-5A22-1C40-93AF-E88E2332E5A4}" name="Focus" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{24AAB514-0DA4-6D41-B622-DFFD00A34E8D}" name="Coverage" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{011D8E6E-C900-7648-8085-2B8D2880B641}" name="Access" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{7C68FF17-2976-BA4E-8999-5A67F8E9B01F}" name="Platform" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{7B36FC73-8715-2F4D-9E5C-5BE540BD7F64}" name="Type" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{2DD0E2CD-5A22-1C40-93AF-E88E2332E5A4}" name="Focus" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{24AAB514-0DA4-6D41-B622-DFFD00A34E8D}" name="Coverage" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{011D8E6E-C900-7648-8085-2B8D2880B641}" name="Access" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{CF4D4718-B4E7-3A42-B0BF-59C582CE5A73}" name="ResultSet1" displayName="ResultSet1" ref="B27:J63" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="B27:J63" xr:uid="{CF4D4718-B4E7-3A42-B0BF-59C582CE5A73}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{3BA4207A-A99E-B44D-9BE0-74DD6117E5EC}" name="Run#" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{A3281DC4-8FBF-EF4F-9FFE-A4C58FF26762}" name="Query#" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{C2731D82-ABF4-5E46-8C6B-197A18BF0363}" name="Date" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{2A0AFBED-E7B6-984C-BA37-7252DBD81F68}" name="Steps taken" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{BCF50AB6-A31F-0342-9657-66F8396C7CDA}" name="Database" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{15AD81DA-35A7-2042-90D3-4002CF594DCC}" name="QueryNr" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{6DA450DF-0BBF-E542-B5B0-173E2A6BB46E}" name="QueryString" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{65D0B927-0C74-FD4F-936E-8325830FDC27}" name="Quantity" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{4C2C5098-15DB-3F47-905E-87A97BAC943F}" name="Notes / Comments" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4799,18 +5094,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6764B6A2-AEB7-C544-9994-5A15BB9C9B07}">
-  <dimension ref="B2:I19"/>
+  <dimension ref="B2:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
     <col min="9" max="9" width="11.5" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
@@ -5028,7 +5326,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="23" t="s">
         <v>166</v>
       </c>
@@ -5045,7 +5343,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="22" t="s">
         <v>167</v>
       </c>
@@ -5062,7 +5360,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="23" t="s">
         <v>36</v>
       </c>
@@ -5079,11 +5377,1061 @@
         <v>194</v>
       </c>
     </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B27" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="H27" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="I27" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="J27" s="27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B28" s="28">
+        <v>1</v>
+      </c>
+      <c r="C28" s="28">
+        <v>1</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="G28" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="H28" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="I28" s="28">
+        <v>1</v>
+      </c>
+      <c r="J28" s="30"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B29" s="6">
+        <v>1</v>
+      </c>
+      <c r="C29" s="6">
+        <v>2</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I29" s="6">
+        <v>0</v>
+      </c>
+      <c r="J29" s="31"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B30" s="28">
+        <v>1</v>
+      </c>
+      <c r="C30" s="28">
+        <v>3</v>
+      </c>
+      <c r="D30" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="E30" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="H30" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I30" s="28">
+        <v>1</v>
+      </c>
+      <c r="J30" s="30"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B31" s="6">
+        <v>1</v>
+      </c>
+      <c r="C31" s="6">
+        <v>4</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I31" s="6">
+        <v>0</v>
+      </c>
+      <c r="J31" s="31"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B32" s="28">
+        <v>1</v>
+      </c>
+      <c r="C32" s="28">
+        <v>5</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="G32" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="H32" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="I32" s="28">
+        <v>0</v>
+      </c>
+      <c r="J32" s="30"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B33" s="6">
+        <v>1</v>
+      </c>
+      <c r="C33" s="6">
+        <v>6</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I33" s="6">
+        <v>59</v>
+      </c>
+      <c r="J33" s="31"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B34" s="28">
+        <v>1</v>
+      </c>
+      <c r="C34" s="28">
+        <v>7</v>
+      </c>
+      <c r="D34" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="G34" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="H34" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="I34" s="28">
+        <v>112</v>
+      </c>
+      <c r="J34" s="30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B35" s="6">
+        <v>1</v>
+      </c>
+      <c r="C35" s="6">
+        <v>8</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I35" s="6">
+        <v>18</v>
+      </c>
+      <c r="J35" s="31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B36" s="28">
+        <v>1</v>
+      </c>
+      <c r="C36" s="28">
+        <v>9</v>
+      </c>
+      <c r="D36" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="G36" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="H36" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="I36" s="28">
+        <v>3</v>
+      </c>
+      <c r="J36" s="30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B37" s="6">
+        <v>1</v>
+      </c>
+      <c r="C37" s="6">
+        <v>10</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I37" s="6">
+        <v>0</v>
+      </c>
+      <c r="J37" s="31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B38" s="28">
+        <v>1</v>
+      </c>
+      <c r="C38" s="28">
+        <v>11</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="E38" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="G38" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="H38" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="I38" s="28">
+        <v>0</v>
+      </c>
+      <c r="J38" s="30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B39" s="6">
+        <v>1</v>
+      </c>
+      <c r="C39" s="6">
+        <v>12</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I39" s="6">
+        <v>929</v>
+      </c>
+      <c r="J39" s="31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B40" s="28">
+        <v>1</v>
+      </c>
+      <c r="C40" s="28">
+        <v>13</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="E40" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="G40" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="H40" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="I40" s="28">
+        <v>0</v>
+      </c>
+      <c r="J40" s="30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B41" s="6">
+        <v>1</v>
+      </c>
+      <c r="C41" s="6">
+        <v>14</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I41" s="6">
+        <v>0</v>
+      </c>
+      <c r="J41" s="31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B42" s="28">
+        <v>1</v>
+      </c>
+      <c r="C42" s="28">
+        <v>15</v>
+      </c>
+      <c r="D42" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="E42" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="G42" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="H42" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="I42" s="28">
+        <v>0</v>
+      </c>
+      <c r="J42" s="30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B43" s="6">
+        <v>1</v>
+      </c>
+      <c r="C43" s="6">
+        <v>16</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I43" s="6">
+        <v>0</v>
+      </c>
+      <c r="J43" s="31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B44" s="28">
+        <v>1</v>
+      </c>
+      <c r="C44" s="28">
+        <v>17</v>
+      </c>
+      <c r="D44" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="E44" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F44" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="G44" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="H44" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="I44" s="28">
+        <v>0</v>
+      </c>
+      <c r="J44" s="30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B45" s="6">
+        <v>1</v>
+      </c>
+      <c r="C45" s="6">
+        <v>18</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I45" s="6">
+        <v>2</v>
+      </c>
+      <c r="J45" s="31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B46" s="28">
+        <v>1</v>
+      </c>
+      <c r="C46" s="28">
+        <v>19</v>
+      </c>
+      <c r="D46" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="E46" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F46" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="G46" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="H46" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="I46" s="28">
+        <v>1</v>
+      </c>
+      <c r="J46" s="30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B47" s="6">
+        <v>1</v>
+      </c>
+      <c r="C47" s="6">
+        <v>20</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I47" s="6">
+        <v>0</v>
+      </c>
+      <c r="J47" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B48" s="28">
+        <v>1</v>
+      </c>
+      <c r="C48" s="28">
+        <v>21</v>
+      </c>
+      <c r="D48" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="E48" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F48" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="G48" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="H48" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="I48" s="28">
+        <v>0</v>
+      </c>
+      <c r="J48" s="30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B49" s="6">
+        <v>1</v>
+      </c>
+      <c r="C49" s="6">
+        <v>22</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I49" s="6">
+        <v>0</v>
+      </c>
+      <c r="J49" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B50" s="28">
+        <v>1</v>
+      </c>
+      <c r="C50" s="28">
+        <v>23</v>
+      </c>
+      <c r="D50" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F50" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="G50" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="H50" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="I50" s="28">
+        <v>0</v>
+      </c>
+      <c r="J50" s="30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B51" s="6">
+        <v>1</v>
+      </c>
+      <c r="C51" s="6">
+        <v>24</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I51" s="6">
+        <v>4</v>
+      </c>
+      <c r="J51" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B52" s="28">
+        <v>1</v>
+      </c>
+      <c r="C52" s="28">
+        <v>25</v>
+      </c>
+      <c r="D52" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="E52" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F52" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="G52" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="H52" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="I52" s="28">
+        <v>4</v>
+      </c>
+      <c r="J52" s="30"/>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B53" s="6">
+        <v>1</v>
+      </c>
+      <c r="C53" s="6">
+        <v>26</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I53" s="6">
+        <v>0</v>
+      </c>
+      <c r="J53" s="31"/>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B54" s="28">
+        <v>1</v>
+      </c>
+      <c r="C54" s="28">
+        <v>27</v>
+      </c>
+      <c r="D54" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="E54" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F54" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="G54" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="H54" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="I54" s="28">
+        <v>2</v>
+      </c>
+      <c r="J54" s="30"/>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B55" s="6">
+        <v>1</v>
+      </c>
+      <c r="C55" s="6">
+        <v>28</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I55" s="6">
+        <v>0</v>
+      </c>
+      <c r="J55" s="31"/>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B56" s="28">
+        <v>1</v>
+      </c>
+      <c r="C56" s="28">
+        <v>29</v>
+      </c>
+      <c r="D56" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="E56" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F56" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="G56" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="H56" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="I56" s="28">
+        <v>1</v>
+      </c>
+      <c r="J56" s="30"/>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B57" s="6">
+        <v>1</v>
+      </c>
+      <c r="C57" s="6">
+        <v>30</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I57" s="6">
+        <v>43</v>
+      </c>
+      <c r="J57" s="31"/>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B58" s="28">
+        <v>1</v>
+      </c>
+      <c r="C58" s="28">
+        <v>31</v>
+      </c>
+      <c r="D58" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="E58" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F58" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="G58" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="H58" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="I58" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="J58" s="30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B59" s="6">
+        <v>1</v>
+      </c>
+      <c r="C59" s="6">
+        <v>32</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I59" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="J59" s="31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B60" s="28">
+        <v>1</v>
+      </c>
+      <c r="C60" s="28">
+        <v>33</v>
+      </c>
+      <c r="D60" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="E60" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F60" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="G60" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="H60" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="I60" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="J60" s="30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B61" s="6">
+        <v>1</v>
+      </c>
+      <c r="C61" s="6">
+        <v>34</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I61" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="J61" s="31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B62" s="28">
+        <v>1</v>
+      </c>
+      <c r="C62" s="28">
+        <v>35</v>
+      </c>
+      <c r="D62" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="E62" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F62" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="G62" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="H62" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="I62" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="J62" s="30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B63" s="6">
+        <v>1</v>
+      </c>
+      <c r="C63" s="6">
+        <v>36</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I63" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="J63" s="31" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated tables and diagrams
</commit_message>
<xml_diff>
--- a/tables/slr_logbook.xlsx
+++ b/tables/slr_logbook.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Projects/literature/phd_kul/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84211482-AE79-EA49-9694-7D54EA3BC3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F46756-87FE-3C43-8FA5-9A44A8499E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37640" yWindow="1620" windowWidth="36160" windowHeight="36180" activeTab="2" xr2:uid="{AC0C9749-44FB-E246-A4D0-62D1F20133DE}"/>
+    <workbookView xWindow="24660" yWindow="1960" windowWidth="36160" windowHeight="36180" activeTab="2" xr2:uid="{AC0C9749-44FB-E246-A4D0-62D1F20133DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
     <sheet name="Pivot" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="Results" sheetId="5" r:id="rId3"/>
     <sheet name="2021" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="207">
   <si>
     <t>Date</t>
   </si>
@@ -577,145 +577,142 @@
     <t>"business process management" and "risk management" and "non financial information"</t>
   </si>
   <si>
-    <t>Platform</t>
-  </si>
-  <si>
-    <t>Web of Science</t>
-  </si>
-  <si>
-    <t>ScienceDirect</t>
-  </si>
-  <si>
-    <t>SSRN</t>
-  </si>
-  <si>
-    <t>arXiv</t>
-  </si>
-  <si>
-    <t>DBLP</t>
-  </si>
-  <si>
-    <t>Zenodo</t>
+    <t>CPAPER</t>
+  </si>
+  <si>
+    <t>Impact of Legal Interpretation on Business Process Compliance</t>
+  </si>
+  <si>
+    <t>JOUR</t>
+  </si>
+  <si>
+    <t>A framework for visually monitoring business process compliance</t>
+  </si>
+  <si>
+    <t>Business Process Compliance Management: An Integrated Proactive Approach</t>
+  </si>
+  <si>
+    <t>Business Process Compliance using Reference Models of Law</t>
+  </si>
+  <si>
+    <t>Formalizing and appling compliance patterns for business process compliance</t>
+  </si>
+  <si>
+    <t>Lifecycle Business Process Compliance Management: A Semantically-Enabled Framework</t>
+  </si>
+  <si>
+    <t>An Anti-Pattern-based Runtime Business Process Compliance Monitoring Framework</t>
+  </si>
+  <si>
+    <t>An Approach Toward the Economic Assessment of Business Process Compliance</t>
+  </si>
+  <si>
+    <t>The influence of directive explanations on users' business process compliance performance</t>
+  </si>
+  <si>
+    <t>Why Do Banks Find Business Process Compliance so Challenging? An Australian Perspective</t>
+  </si>
+  <si>
+    <t>Design-time business process compliance assessment based on multi-granularity semantic information</t>
+  </si>
+  <si>
+    <t>Runtime Detection of Business Process Compliance Violations: An Approach based on Anti Patterns</t>
+  </si>
+  <si>
+    <t>An Experience Report of Improving Business Process Compliance Using Security Risk-Oriented Patterns</t>
+  </si>
+  <si>
+    <t>A Taxonomy of Business Rule Organizing Approaches in Regard to Business Process Compliance</t>
+  </si>
+  <si>
+    <t>Collection and Elicitation of Business Process Compliance Patterns with Focus on Data Aspects</t>
+  </si>
+  <si>
+    <t>Are we done with business process compliance: state of the art and challenges ahead</t>
+  </si>
+  <si>
+    <t>Towards Supporting Business Process Compliance Checking with Compliance Pattern Catalogues A Financial Industry Case Study</t>
+  </si>
+  <si>
+    <t>A Model-based Business Process Compliance Management Architecture for SMSE towards Effective Adoption of Cloud Computing</t>
+  </si>
+  <si>
+    <t>Business process compliance checking - applying and evaluating a generic pattern matching approach for conceptual models in the financial sector</t>
   </si>
   <si>
     <t>Type</t>
   </si>
   <si>
-    <t>Citation index</t>
-  </si>
-  <si>
-    <t>Academic literature platform</t>
-  </si>
-  <si>
-    <t>Preprints</t>
-  </si>
-  <si>
-    <t>Bibliography database</t>
-  </si>
-  <si>
-    <t>Dataset repository</t>
-  </si>
-  <si>
-    <t>Knowledge base</t>
-  </si>
-  <si>
-    <t>Focus</t>
-  </si>
-  <si>
-    <t>Wide range of disciplines (including hard sciences, social sciences, and the humanities)</t>
-  </si>
-  <si>
-    <t>Science, technology, medicine, and social science</t>
-  </si>
-  <si>
-    <t>Social sciences, economics, and business</t>
-  </si>
-  <si>
-    <t>Hard sciences and quantitative sciences</t>
-  </si>
-  <si>
-    <t>Computer science</t>
-  </si>
-  <si>
-    <t>Data from various disciplines</t>
-  </si>
-  <si>
-    <t>Academic publications and research outputs</t>
-  </si>
-  <si>
-    <t>Coverage</t>
-  </si>
-  <si>
-    <t>Over 18,000 academic journals, books, patents, and other scholarly publications</t>
-  </si>
-  <si>
-    <t>Over 3,500 peer-reviewed journals</t>
-  </si>
-  <si>
-    <t>Early-stage social science, economics, and business research papers</t>
-  </si>
-  <si>
-    <t>Early-stage research papers in a wide range of disciplines</t>
-  </si>
-  <si>
-    <t>Scholarly publications in computer science</t>
-  </si>
-  <si>
-    <t>Data from research projects, surveys, and other data collection efforts</t>
-  </si>
-  <si>
-    <t>Academic publications and research outputs from universities, research institutions, and scholarly societies</t>
-  </si>
-  <si>
-    <t>Access</t>
-  </si>
-  <si>
-    <t>Subscription-based</t>
-  </si>
-  <si>
-    <t>Subscription-based and open access</t>
-  </si>
-  <si>
-    <t>Open access</t>
-  </si>
-  <si>
-    <t>Run#</t>
-  </si>
-  <si>
-    <t>Query#</t>
-  </si>
-  <si>
-    <t>11/24/2023</t>
-  </si>
-  <si>
-    <t>Q01</t>
-  </si>
-  <si>
-    <t>Q02</t>
-  </si>
-  <si>
-    <t>Q03</t>
-  </si>
-  <si>
-    <t>Q04</t>
-  </si>
-  <si>
-    <t>Q05</t>
-  </si>
-  <si>
-    <t>Q06</t>
-  </si>
-  <si>
-    <t>dblp</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>7</t>
+    <t>Nr</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Blockchain-as-a-Service for Business Process Management: Survey and Challenges</t>
+  </si>
+  <si>
+    <t>Managing Security Objects and -Processes Using an Extended BPM Approach and -System</t>
+  </si>
+  <si>
+    <t>Business Process Management - A Traditional Approach versus a Knowledge Based Approach</t>
+  </si>
+  <si>
+    <t>Toward agile Business Process Management: Description of concepts and a proposed definition</t>
+  </si>
+  <si>
+    <t>Spreadsheets for business process management Using process mining to deal with "events" rather than "numbers"?</t>
+  </si>
+  <si>
+    <t>BPM perspectives to support ICSs: Exploiting the integration of formal verifications into investment service provision processes</t>
+  </si>
+  <si>
+    <t>Improved Compliance by BPM-Driven Workflow Automation</t>
+  </si>
+  <si>
+    <t>Simulation of the Inventory Process in a Postharvest of Export Roses Under a Business Process Management approach</t>
+  </si>
+  <si>
+    <t>BPM analysis and security case study: dining rooms Cartagena military, Colombia</t>
+  </si>
+  <si>
+    <t>The influence of BPM-supportive culture and individual process orientation on process conformance</t>
+  </si>
+  <si>
+    <t>Semi-automated checking for regulatory compliance in e-Health</t>
+  </si>
+  <si>
+    <t>Blockchain-based business process management (BPM) framework for service composition in industry 4.0</t>
+  </si>
+  <si>
+    <t>BUSINESS PROCESS MANAGEMENT DRIVEN BY DATA GOVERNANCE</t>
+  </si>
+  <si>
+    <t>An Open-Source Proactive Security Infrastructure For Business Process Management</t>
+  </si>
+  <si>
+    <t>Cloud Based Privacy Preserving Collaborative Business Process Management</t>
+  </si>
+  <si>
+    <t>A knowledge-intensive adaptive business process management framework</t>
+  </si>
+  <si>
+    <t>Process model verifier for integrated medical healthcare systems using business process management system</t>
+  </si>
+  <si>
+    <t>Agile Innovation Through Business Process Management: Realizing the Potential of Digital Transformation</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
   </si>
 </sst>
 </file>
@@ -726,7 +723,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -790,27 +787,21 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -829,12 +820,6 @@
         <bgColor rgb="FFD9E1F2"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -848,7 +833,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FF8EA9DB"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -859,7 +844,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -891,67 +876,18 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF4472C4"/>
-          <bgColor rgb="FF4472C4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <font>
         <b val="0"/>
@@ -963,64 +899,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="Calibri"/>
         <family val="2"/>
@@ -1038,45 +917,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="Calibri"/>
         <family val="2"/>
@@ -1094,89 +935,8 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1193,8 +953,26 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1203,7 +981,7 @@
         <left/>
         <right/>
         <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
+          <color rgb="FF8EA9DB"/>
         </top>
         <bottom/>
         <vertical/>
@@ -1221,138 +999,12 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1365,11 +1017,11 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Arial"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
         <family val="2"/>
-        <scheme val="none"/>
+        <scheme val="minor"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -1377,7 +1029,6 @@
           <bgColor rgb="FF4472C4"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
     </dxf>
     <dxf>
       <alignment horizontal="right"/>
@@ -2320,17 +1971,17 @@
     <dataField name="Sum of Quantity" fld="7" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="23">
+    <format dxfId="9">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -2347,67 +1998,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FFF0228E-16A0-0745-BA5A-B606859071BD}" name="Table1" displayName="Table1" ref="A7:I73" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FFF0228E-16A0-0745-BA5A-B606859071BD}" name="Table1" displayName="Table1" ref="A7:I73" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A7:I73" xr:uid="{FFF0228E-16A0-0745-BA5A-B606859071BD}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{ABE8919E-31E3-3C4D-BE26-E0B097FD8BAF}" name="Record" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{DCEAF83F-13E5-F04F-959B-309C1258F8D6}" name="Date" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{7D890402-E0DD-7941-A452-A014F2CD93DD}" name="Steps taken" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{32C6624E-63B0-B64B-AB39-6467D72B490D}" name="Database" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{8C094E55-9E0E-FC42-9895-83D32CEF90A9}" name="QueryNr" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{2FFD36BC-A2D2-A848-868B-212869119555}" name="QuerySubNr" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{ABE8919E-31E3-3C4D-BE26-E0B097FD8BAF}" name="Record" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{DCEAF83F-13E5-F04F-959B-309C1258F8D6}" name="Date" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{7D890402-E0DD-7941-A452-A014F2CD93DD}" name="Steps taken" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{32C6624E-63B0-B64B-AB39-6467D72B490D}" name="Database" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{8C094E55-9E0E-FC42-9895-83D32CEF90A9}" name="QueryNr" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{2FFD36BC-A2D2-A848-868B-212869119555}" name="QuerySubNr" dataDxfId="12"/>
     <tableColumn id="7" xr3:uid="{762D1B3E-C5F1-6D43-B97F-55EAA8FDB56C}" name="QueryString"/>
-    <tableColumn id="8" xr3:uid="{0E1EDC8C-20E2-CF43-9DE7-56E7C0BF256D}" name="Quantity" dataDxfId="25"/>
-    <tableColumn id="9" xr3:uid="{92D1697A-99F2-814E-A00C-ED758147A27A}" name="Notes / Comments" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{0E1EDC8C-20E2-CF43-9DE7-56E7C0BF256D}" name="Quantity" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{92D1697A-99F2-814E-A00C-ED758147A27A}" name="Notes / Comments" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A20822EB-39FA-6648-9837-2FAF2BBFC395}" name="Databases" displayName="Databases" ref="B2:I6" totalsRowShown="0" headerRowDxfId="20" tableBorderDxfId="19">
-  <autoFilter ref="B2:I6" xr:uid="{A20822EB-39FA-6648-9837-2FAF2BBFC395}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F4EF182A-30AC-754D-86FF-2E2ADCC705E9}" name="Platform"/>
-    <tableColumn id="2" xr3:uid="{56E9FBF2-2994-2748-B295-3DB88B2EDDD5}" name="Web of Science"/>
-    <tableColumn id="3" xr3:uid="{B0EF25B1-0375-C640-88C9-873752774E62}" name="ScienceDirect"/>
-    <tableColumn id="4" xr3:uid="{C76BBAAB-83F0-214C-9B08-4A1790A46529}" name="SSRN"/>
-    <tableColumn id="5" xr3:uid="{97018384-0991-9346-A86B-ECB7C17EF056}" name="arXiv"/>
-    <tableColumn id="6" xr3:uid="{47735B29-3713-604E-9ED9-F319585CB371}" name="DBLP"/>
-    <tableColumn id="7" xr3:uid="{0CAE628A-3842-C748-82DF-321D3A36E786}" name="Zenodo"/>
-    <tableColumn id="8" xr3:uid="{AAA42901-B756-6C47-93E9-9689444E6690}" name="OpenAlex"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{85AFCCCA-7255-F341-BACF-D289839D2415}" name="Database2" displayName="Database2" ref="B12:F19" totalsRowShown="0" headerRowDxfId="11" dataDxfId="12" tableBorderDxfId="18">
-  <autoFilter ref="B12:F19" xr:uid="{85AFCCCA-7255-F341-BACF-D289839D2415}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6E9493DF-B8FF-814B-80AF-65E187D50930}" name="ResultSet" displayName="ResultSet" ref="A1:E48" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E48" xr:uid="{6E9493DF-B8FF-814B-80AF-65E187D50930}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7C68FF17-2976-BA4E-8999-5A67F8E9B01F}" name="Platform" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{7B36FC73-8715-2F4D-9E5C-5BE540BD7F64}" name="Type" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{2DD0E2CD-5A22-1C40-93AF-E88E2332E5A4}" name="Focus" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{24AAB514-0DA4-6D41-B622-DFFD00A34E8D}" name="Coverage" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{011D8E6E-C900-7648-8085-2B8D2880B641}" name="Access" dataDxfId="13"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{CF4D4718-B4E7-3A42-B0BF-59C582CE5A73}" name="ResultSet1" displayName="ResultSet1" ref="B27:J63" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="B27:J63" xr:uid="{CF4D4718-B4E7-3A42-B0BF-59C582CE5A73}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{3BA4207A-A99E-B44D-9BE0-74DD6117E5EC}" name="Run#" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{A3281DC4-8FBF-EF4F-9FFE-A4C58FF26762}" name="Query#" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{C2731D82-ABF4-5E46-8C6B-197A18BF0363}" name="Date" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{2A0AFBED-E7B6-984C-BA37-7252DBD81F68}" name="Steps taken" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{BCF50AB6-A31F-0342-9657-66F8396C7CDA}" name="Database" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{15AD81DA-35A7-2042-90D3-4002CF594DCC}" name="QueryNr" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{6DA450DF-0BBF-E542-B5B0-173E2A6BB46E}" name="QueryString" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{65D0B927-0C74-FD4F-936E-8325830FDC27}" name="Quantity" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{4C2C5098-15DB-3F47-905E-87A97BAC943F}" name="Notes / Comments" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{002D061F-1517-4947-B3DF-0195A61509C4}" name="Nr" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{75299883-CBB7-B443-BB79-6C66D7D5D7C4}" name="Type" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{E62766D9-866F-F546-84DB-31F350AE6381}" name="Title" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{2FCBFE5D-B31B-7A4D-9464-517BCCE3DBE9}" name="Select" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{EBB80226-63B9-F24F-A24D-CE2EEDDC3724}" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5094,1344 +4710,666 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6764B6A2-AEB7-C544-9994-5A15BB9C9B07}">
-  <dimension ref="B2:J63"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" customWidth="1"/>
-    <col min="9" max="9" width="11.5" customWidth="1"/>
-    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="113.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="21" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="19">
+        <v>1</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="20">
+        <v>2</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="C3" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="22">
+        <v>3</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="20">
+        <v>4</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="22">
+        <v>5</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="20">
+        <v>6</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="22">
+        <v>7</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="20">
+        <v>8</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="22">
+        <v>9</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="20">
+        <v>10</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="E11" s="20"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="22">
+        <v>11</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="20">
+        <v>12</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="22">
+        <v>13</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="20">
+        <v>14</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="22">
+        <v>15</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="20">
+        <v>16</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="22">
+        <v>17</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="20">
+        <v>18</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="22">
+        <v>19</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="20">
+        <v>20</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="20">
+        <v>22</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="22">
+        <v>23</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="20">
+        <v>24</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="22">
+        <v>25</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="20">
+        <v>26</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="E27" s="20"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="22">
+        <v>27</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="20">
+        <v>28</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="22">
+        <v>29</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="20">
+        <v>30</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="E31" s="20"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="22">
+        <v>31</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="20">
+        <v>32</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="E33" s="20"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="22">
+        <v>33</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="20">
+        <v>34</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="22">
+        <v>35</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="20">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="I4" s="20" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="D5" s="19" t="s">
+      <c r="B37" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="22">
+        <v>37</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="20">
+        <v>38</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C39" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="22">
+        <v>39</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C40" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="20">
+        <v>40</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C41" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="22">
+        <v>41</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C42" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="20">
+        <v>42</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C43" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="D43" s="20"/>
+      <c r="E43" s="20" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="22">
+        <v>43</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C44" s="21" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="20" t="s">
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="20">
+        <v>44</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C45" s="20" t="s">
         <v>191</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="D45" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="E45" s="20" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="22">
+        <v>45</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C46" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="20">
+        <v>46</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C47" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="22">
+        <v>47</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C48" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="F6" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="I6" s="20" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>175</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>183</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>177</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="22" t="s">
-        <v>165</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="F16" s="22" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>172</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>173</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="F18" s="22" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B27" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="E27" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="G27" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="H27" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="I27" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="J27" s="27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B28" s="28">
-        <v>1</v>
-      </c>
-      <c r="C28" s="28">
-        <v>1</v>
-      </c>
-      <c r="D28" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="G28" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="H28" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="I28" s="28">
-        <v>1</v>
-      </c>
-      <c r="J28" s="30"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="6">
-        <v>1</v>
-      </c>
-      <c r="C29" s="6">
-        <v>2</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I29" s="6">
-        <v>0</v>
-      </c>
-      <c r="J29" s="31"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B30" s="28">
-        <v>1</v>
-      </c>
-      <c r="C30" s="28">
-        <v>3</v>
-      </c>
-      <c r="D30" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E30" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F30" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="G30" s="28" t="s">
-        <v>200</v>
-      </c>
-      <c r="H30" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="I30" s="28">
-        <v>1</v>
-      </c>
-      <c r="J30" s="30"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B31" s="6">
-        <v>1</v>
-      </c>
-      <c r="C31" s="6">
-        <v>4</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I31" s="6">
-        <v>0</v>
-      </c>
-      <c r="J31" s="31"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B32" s="28">
-        <v>1</v>
-      </c>
-      <c r="C32" s="28">
-        <v>5</v>
-      </c>
-      <c r="D32" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E32" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F32" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="G32" s="28" t="s">
-        <v>202</v>
-      </c>
-      <c r="H32" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="I32" s="28">
-        <v>0</v>
-      </c>
-      <c r="J32" s="30"/>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B33" s="6">
-        <v>1</v>
-      </c>
-      <c r="C33" s="6">
-        <v>6</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I33" s="6">
-        <v>59</v>
-      </c>
-      <c r="J33" s="31"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B34" s="28">
-        <v>1</v>
-      </c>
-      <c r="C34" s="28">
-        <v>7</v>
-      </c>
-      <c r="D34" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E34" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F34" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="G34" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="H34" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="I34" s="28">
-        <v>112</v>
-      </c>
-      <c r="J34" s="30" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B35" s="6">
-        <v>1</v>
-      </c>
-      <c r="C35" s="6">
-        <v>8</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="I35" s="6">
-        <v>18</v>
-      </c>
-      <c r="J35" s="31" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B36" s="28">
-        <v>1</v>
-      </c>
-      <c r="C36" s="28">
-        <v>9</v>
-      </c>
-      <c r="D36" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E36" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F36" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="G36" s="28" t="s">
-        <v>200</v>
-      </c>
-      <c r="H36" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="I36" s="28">
-        <v>3</v>
-      </c>
-      <c r="J36" s="30" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B37" s="6">
-        <v>1</v>
-      </c>
-      <c r="C37" s="6">
-        <v>10</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I37" s="6">
-        <v>0</v>
-      </c>
-      <c r="J37" s="31" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B38" s="28">
-        <v>1</v>
-      </c>
-      <c r="C38" s="28">
-        <v>11</v>
-      </c>
-      <c r="D38" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E38" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F38" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="G38" s="28" t="s">
-        <v>202</v>
-      </c>
-      <c r="H38" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="I38" s="28">
-        <v>0</v>
-      </c>
-      <c r="J38" s="30" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B39" s="6">
-        <v>1</v>
-      </c>
-      <c r="C39" s="6">
-        <v>12</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I39" s="6">
-        <v>929</v>
-      </c>
-      <c r="J39" s="31" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B40" s="28">
-        <v>1</v>
-      </c>
-      <c r="C40" s="28">
-        <v>13</v>
-      </c>
-      <c r="D40" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E40" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F40" s="28" t="s">
-        <v>164</v>
-      </c>
-      <c r="G40" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="H40" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="I40" s="28">
-        <v>0</v>
-      </c>
-      <c r="J40" s="30" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B41" s="6">
-        <v>1</v>
-      </c>
-      <c r="C41" s="6">
-        <v>14</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I41" s="6">
-        <v>0</v>
-      </c>
-      <c r="J41" s="31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B42" s="28">
-        <v>1</v>
-      </c>
-      <c r="C42" s="28">
-        <v>15</v>
-      </c>
-      <c r="D42" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E42" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F42" s="28" t="s">
-        <v>164</v>
-      </c>
-      <c r="G42" s="28" t="s">
-        <v>200</v>
-      </c>
-      <c r="H42" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="I42" s="28">
-        <v>0</v>
-      </c>
-      <c r="J42" s="30" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B43" s="6">
-        <v>1</v>
-      </c>
-      <c r="C43" s="6">
-        <v>16</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="I43" s="6">
-        <v>0</v>
-      </c>
-      <c r="J43" s="31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B44" s="28">
-        <v>1</v>
-      </c>
-      <c r="C44" s="28">
-        <v>17</v>
-      </c>
-      <c r="D44" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E44" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F44" s="28" t="s">
-        <v>164</v>
-      </c>
-      <c r="G44" s="28" t="s">
-        <v>202</v>
-      </c>
-      <c r="H44" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="I44" s="28">
-        <v>0</v>
-      </c>
-      <c r="J44" s="30" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B45" s="6">
-        <v>1</v>
-      </c>
-      <c r="C45" s="6">
-        <v>18</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="G45" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I45" s="6">
-        <v>2</v>
-      </c>
-      <c r="J45" s="31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B46" s="28">
-        <v>1</v>
-      </c>
-      <c r="C46" s="28">
-        <v>19</v>
-      </c>
-      <c r="D46" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E46" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F46" s="28" t="s">
-        <v>165</v>
-      </c>
-      <c r="G46" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="H46" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="I46" s="28">
-        <v>1</v>
-      </c>
-      <c r="J46" s="30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B47" s="6">
-        <v>1</v>
-      </c>
-      <c r="C47" s="6">
-        <v>20</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I47" s="6">
-        <v>0</v>
-      </c>
-      <c r="J47" s="31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B48" s="28">
-        <v>1</v>
-      </c>
-      <c r="C48" s="28">
-        <v>21</v>
-      </c>
-      <c r="D48" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E48" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F48" s="28" t="s">
-        <v>165</v>
-      </c>
-      <c r="G48" s="28" t="s">
-        <v>200</v>
-      </c>
-      <c r="H48" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="I48" s="28">
-        <v>0</v>
-      </c>
-      <c r="J48" s="30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B49" s="6">
-        <v>1</v>
-      </c>
-      <c r="C49" s="6">
-        <v>22</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="I49" s="6">
-        <v>0</v>
-      </c>
-      <c r="J49" s="31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B50" s="28">
-        <v>1</v>
-      </c>
-      <c r="C50" s="28">
-        <v>23</v>
-      </c>
-      <c r="D50" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E50" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F50" s="28" t="s">
-        <v>165</v>
-      </c>
-      <c r="G50" s="28" t="s">
-        <v>202</v>
-      </c>
-      <c r="H50" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="I50" s="28">
-        <v>0</v>
-      </c>
-      <c r="J50" s="30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B51" s="6">
-        <v>1</v>
-      </c>
-      <c r="C51" s="6">
-        <v>24</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I51" s="6">
-        <v>4</v>
-      </c>
-      <c r="J51" s="31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B52" s="28">
-        <v>1</v>
-      </c>
-      <c r="C52" s="28">
-        <v>25</v>
-      </c>
-      <c r="D52" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E52" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F52" s="28" t="s">
-        <v>204</v>
-      </c>
-      <c r="G52" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="H52" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="I52" s="28">
-        <v>4</v>
-      </c>
-      <c r="J52" s="30"/>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B53" s="6">
-        <v>1</v>
-      </c>
-      <c r="C53" s="6">
-        <v>26</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="G53" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="H53" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I53" s="6">
-        <v>0</v>
-      </c>
-      <c r="J53" s="31"/>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B54" s="28">
-        <v>1</v>
-      </c>
-      <c r="C54" s="28">
-        <v>27</v>
-      </c>
-      <c r="D54" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E54" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F54" s="28" t="s">
-        <v>204</v>
-      </c>
-      <c r="G54" s="28" t="s">
-        <v>200</v>
-      </c>
-      <c r="H54" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="I54" s="28">
-        <v>2</v>
-      </c>
-      <c r="J54" s="30"/>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B55" s="6">
-        <v>1</v>
-      </c>
-      <c r="C55" s="6">
-        <v>28</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="G55" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="H55" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="I55" s="6">
-        <v>0</v>
-      </c>
-      <c r="J55" s="31"/>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B56" s="28">
-        <v>1</v>
-      </c>
-      <c r="C56" s="28">
-        <v>29</v>
-      </c>
-      <c r="D56" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E56" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F56" s="28" t="s">
-        <v>204</v>
-      </c>
-      <c r="G56" s="28" t="s">
-        <v>202</v>
-      </c>
-      <c r="H56" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="I56" s="28">
-        <v>1</v>
-      </c>
-      <c r="J56" s="30"/>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B57" s="6">
-        <v>1</v>
-      </c>
-      <c r="C57" s="6">
-        <v>30</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I57" s="6">
-        <v>43</v>
-      </c>
-      <c r="J57" s="31"/>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B58" s="28">
-        <v>1</v>
-      </c>
-      <c r="C58" s="28">
-        <v>31</v>
-      </c>
-      <c r="D58" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E58" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F58" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="G58" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="H58" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="I58" s="28" t="s">
-        <v>205</v>
-      </c>
-      <c r="J58" s="30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B59" s="6">
-        <v>1</v>
-      </c>
-      <c r="C59" s="6">
-        <v>32</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="G59" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="H59" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="I59" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="J59" s="31" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B60" s="28">
-        <v>1</v>
-      </c>
-      <c r="C60" s="28">
-        <v>33</v>
-      </c>
-      <c r="D60" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E60" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F60" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="G60" s="28" t="s">
-        <v>200</v>
-      </c>
-      <c r="H60" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="I60" s="28" t="s">
-        <v>206</v>
-      </c>
-      <c r="J60" s="30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B61" s="6">
-        <v>1</v>
-      </c>
-      <c r="C61" s="6">
-        <v>34</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="G61" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="H61" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="I61" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="J61" s="31" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B62" s="28">
-        <v>1</v>
-      </c>
-      <c r="C62" s="28">
-        <v>35</v>
-      </c>
-      <c r="D62" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E62" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F62" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="G62" s="28" t="s">
-        <v>202</v>
-      </c>
-      <c r="H62" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="I62" s="28" t="s">
-        <v>206</v>
-      </c>
-      <c r="J62" s="30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B63" s="6">
-        <v>1</v>
-      </c>
-      <c r="C63" s="6">
-        <v>36</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="G63" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="H63" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I63" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="J63" s="31" t="s">
-        <v>24</v>
-      </c>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="3">
+  <tableParts count="1">
     <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Changed project to book
</commit_message>
<xml_diff>
--- a/tables/slr_logbook.xlsx
+++ b/tables/slr_logbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Projects/literature/phd_kul/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8BDD63-9AD0-B749-8844-0E267BA9A845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9DECB5-04CB-F845-9934-59B9F6197480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36120" yWindow="500" windowWidth="35420" windowHeight="36980" activeTab="1" xr2:uid="{AC0C9749-44FB-E246-A4D0-62D1F20133DE}"/>
+    <workbookView xWindow="36120" yWindow="500" windowWidth="38120" windowHeight="41300" activeTab="1" xr2:uid="{AC0C9749-44FB-E246-A4D0-62D1F20133DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="384">
   <si>
     <t>Date</t>
   </si>
@@ -1258,6 +1258,9 @@
   </si>
   <si>
     <t>Business Process and Business Rule Modeling Languages for Compliance Management: A Representational Analysis</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -1384,7 +1387,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1427,13 +1430,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1470,22 +1491,48 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="36">
     <dxf>
       <font>
         <b val="0"/>
@@ -1503,6 +1550,474 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4472C4"/>
+          <bgColor rgb="FF4472C4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4472C4"/>
+          <bgColor rgb="FF4472C4"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1597,6 +2112,24 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -1663,32 +2196,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FFF0228E-16A0-0745-BA5A-B606859071BD}" name="Table1" displayName="Table1" ref="A7:I73" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FFF0228E-16A0-0745-BA5A-B606859071BD}" name="Table1" displayName="Table1" ref="A7:I73" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A7:I73" xr:uid="{FFF0228E-16A0-0745-BA5A-B606859071BD}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{ABE8919E-31E3-3C4D-BE26-E0B097FD8BAF}" name="Record" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{DCEAF83F-13E5-F04F-959B-309C1258F8D6}" name="Date" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{7D890402-E0DD-7941-A452-A014F2CD93DD}" name="Steps taken" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{32C6624E-63B0-B64B-AB39-6467D72B490D}" name="Database" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{8C094E55-9E0E-FC42-9895-83D32CEF90A9}" name="QueryNr" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{2FFD36BC-A2D2-A848-868B-212869119555}" name="QuerySubNr" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{ABE8919E-31E3-3C4D-BE26-E0B097FD8BAF}" name="Record" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{DCEAF83F-13E5-F04F-959B-309C1258F8D6}" name="Date" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{7D890402-E0DD-7941-A452-A014F2CD93DD}" name="Steps taken" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{32C6624E-63B0-B64B-AB39-6467D72B490D}" name="Database" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{8C094E55-9E0E-FC42-9895-83D32CEF90A9}" name="QueryNr" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{2FFD36BC-A2D2-A848-868B-212869119555}" name="QuerySubNr" dataDxfId="28"/>
     <tableColumn id="7" xr3:uid="{762D1B3E-C5F1-6D43-B97F-55EAA8FDB56C}" name="QueryString"/>
-    <tableColumn id="8" xr3:uid="{0E1EDC8C-20E2-CF43-9DE7-56E7C0BF256D}" name="Quantity" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{92D1697A-99F2-814E-A00C-ED758147A27A}" name="Notes / Comments" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{0E1EDC8C-20E2-CF43-9DE7-56E7C0BF256D}" name="Quantity" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{92D1697A-99F2-814E-A00C-ED758147A27A}" name="Notes / Comments" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6E9493DF-B8FF-814B-80AF-65E187D50930}" name="ResultSet" displayName="ResultSet" ref="A1:E91" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E91" xr:uid="{6E9493DF-B8FF-814B-80AF-65E187D50930}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6E9493DF-B8FF-814B-80AF-65E187D50930}" name="database_search" displayName="database_search" ref="A1:E85" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="A1:E85" xr:uid="{6E9493DF-B8FF-814B-80AF-65E187D50930}"/>
   <tableColumns count="5">
-    <tableColumn id="7" xr3:uid="{0D63F18F-F4D2-564D-85E7-1B5B03A3ACFC}" name="Nr." dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{23C1FEFF-7184-2D44-BD2E-CE51BCE64F41}" name="Source" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{75299883-CBB7-B443-BB79-6C66D7D5D7C4}" name="Type" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{E62766D9-866F-F546-84DB-31F350AE6381}" name="Title" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{C76FCD0C-74ED-8A4E-8993-0DCF1F712943}" name="E/I" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{0D63F18F-F4D2-564D-85E7-1B5B03A3ACFC}" name="Nr." dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{23C1FEFF-7184-2D44-BD2E-CE51BCE64F41}" name="Source" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{75299883-CBB7-B443-BB79-6C66D7D5D7C4}" name="Type" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{E62766D9-866F-F546-84DB-31F350AE6381}" name="Title" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{C76FCD0C-74ED-8A4E-8993-0DCF1F712943}" name="E/I" dataDxfId="19"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9B8490AA-2C2C-5147-A986-50BC3AB80588}" name="other_sources" displayName="other_sources" ref="A90:E96" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="A90:E96" xr:uid="{9B8490AA-2C2C-5147-A986-50BC3AB80588}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{74FA861E-AB1E-4347-B062-1242323459F4}" name="Nr." dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{730C5050-4713-6040-9BAA-D73A729DE82B}" name="Source" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{7F733155-80B4-B44C-A594-2E28F6B8D58A}" name="Type" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{1D7C548B-3F49-3F48-BF91-276F5F10A983}" name="Title" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{1922C823-369C-494E-B3F7-4DC76B562B38}" name="E/I" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A9083270-6B7E-EF49-A7D1-0A378430590F}" name="journal_articles" displayName="journal_articles" ref="A100:E125" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="A100:E125" xr:uid="{A9083270-6B7E-EF49-A7D1-0A378430590F}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{6CD914FF-AAFB-0E45-B98A-6AFC1C9DCCE1}" name="Nr." dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{52E2DFDC-BF63-5C46-B657-5E8CBA38A9B5}" name="Source" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{FDB00E17-91CE-B74D-A3DF-B7CDE931522A}" name="Type" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{EE9F59F6-0853-EF4B-A71C-AB7B399BB3D7}" name="Title" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{BD0FCD37-E301-4B4F-9923-2D8E769FDD2F}" name="E/I" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4135,10 +4696,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6764B6A2-AEB7-C544-9994-5A15BB9C9B07}">
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:K125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100:E125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4148,10 +4709,11 @@
     <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="129.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="79" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.5" customWidth="1"/>
+    <col min="10" max="10" width="79" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>295</v>
       </c>
@@ -4167,12 +4729,12 @@
       <c r="E1" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="I1" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="H1" s="16"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="16"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -4188,9 +4750,9 @@
       <c r="E2" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G2" s="16"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -4206,10 +4768,10 @@
       <c r="E3" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -4225,10 +4787,10 @@
       <c r="E4" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -4244,17 +4806,17 @@
       <c r="E5" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="I5" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="J5" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="I5" s="29" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K5" s="27" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -4270,17 +4832,17 @@
       <c r="E6" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="I6" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="J6" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="I6" s="27" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K6" s="25" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -4296,17 +4858,17 @@
       <c r="E7" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="I7" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="H7" s="28" t="s">
+      <c r="J7" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="I7" s="29" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K7" s="27" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
         <v>7</v>
       </c>
@@ -4322,17 +4884,17 @@
       <c r="E8" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="I8" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="J8" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="I8" s="27" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K8" s="25" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
         <v>8</v>
       </c>
@@ -4348,17 +4910,17 @@
       <c r="E9" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="I9" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="H9" s="28" t="s">
+      <c r="J9" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="I9" s="29" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K9" s="27" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="18">
         <v>9</v>
       </c>
@@ -4374,17 +4936,17 @@
       <c r="E10" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G10" s="26" t="s">
+      <c r="I10" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="H10" s="26" t="s">
+      <c r="J10" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="I10" s="27" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K10" s="25" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="18">
         <v>10</v>
       </c>
@@ -4400,17 +4962,17 @@
       <c r="E11" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="I11" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="H11" s="28" t="s">
+      <c r="J11" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="I11" s="29" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K11" s="27" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="18">
         <v>11</v>
       </c>
@@ -4426,17 +4988,17 @@
       <c r="E12" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="G12" s="26" t="s">
+      <c r="I12" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="H12" s="26" t="s">
+      <c r="J12" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="I12" s="27" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K12" s="25" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
         <v>12</v>
       </c>
@@ -4452,17 +5014,17 @@
       <c r="E13" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G13" s="28" t="s">
+      <c r="I13" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="H13" s="28" t="s">
+      <c r="J13" s="26" t="s">
         <v>196</v>
       </c>
-      <c r="I13" s="29" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K13" s="27" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
         <v>13</v>
       </c>
@@ -4478,17 +5040,17 @@
       <c r="E14" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G14" s="26" t="s">
+      <c r="I14" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="H14" s="26" t="s">
+      <c r="J14" s="24" t="s">
         <v>180</v>
       </c>
-      <c r="I14" s="27" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K14" s="25" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
         <v>14</v>
       </c>
@@ -4504,17 +5066,17 @@
       <c r="E15" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G15" s="28" t="s">
+      <c r="I15" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="H15" s="28" t="s">
+      <c r="J15" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="I15" s="29" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K15" s="27" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <v>15</v>
       </c>
@@ -4530,17 +5092,17 @@
       <c r="E16" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G16" s="26" t="s">
+      <c r="I16" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="H16" s="26" t="s">
+      <c r="J16" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="I16" s="27" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K16" s="25" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="18">
         <v>16</v>
       </c>
@@ -4556,9 +5118,9 @@
       <c r="E17" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G17" s="16"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I17" s="16"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="18">
         <v>17</v>
       </c>
@@ -4574,9 +5136,9 @@
       <c r="E18" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G18" s="16"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I18" s="16"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="18">
         <v>18</v>
       </c>
@@ -4592,9 +5154,9 @@
       <c r="E19" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="G19" s="16"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I19" s="16"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="18">
         <v>19</v>
       </c>
@@ -4610,9 +5172,9 @@
       <c r="E20" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="G20" s="16"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I20" s="16"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
         <v>20</v>
       </c>
@@ -4628,9 +5190,9 @@
       <c r="E21" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="G21" s="16"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I21" s="16"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
         <v>21</v>
       </c>
@@ -4646,9 +5208,9 @@
       <c r="E22" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="G22" s="16"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I22" s="16"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
         <v>22</v>
       </c>
@@ -4664,9 +5226,9 @@
       <c r="E23" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="G23" s="16"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I23" s="16"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
         <v>23</v>
       </c>
@@ -4682,9 +5244,9 @@
       <c r="E24" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G24" s="16"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I24" s="16"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="18">
         <v>24</v>
       </c>
@@ -4700,9 +5262,9 @@
       <c r="E25" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G25" s="16"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I25" s="16"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="18">
         <v>25</v>
       </c>
@@ -4718,11 +5280,11 @@
       <c r="E26" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="G26" s="16" t="s">
+      <c r="I26" s="16" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="18">
         <v>26</v>
       </c>
@@ -4738,9 +5300,9 @@
       <c r="E27" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G27" s="16"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I27" s="16"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="18">
         <v>27</v>
       </c>
@@ -4756,9 +5318,9 @@
       <c r="E28" s="16" t="s">
         <v>264</v>
       </c>
-      <c r="G28" s="16"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I28" s="16"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="18">
         <v>28</v>
       </c>
@@ -4774,9 +5336,9 @@
       <c r="E29" s="16" t="s">
         <v>264</v>
       </c>
-      <c r="G29" s="16"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I29" s="16"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="18">
         <v>29</v>
       </c>
@@ -4792,9 +5354,9 @@
       <c r="E30" s="16" t="s">
         <v>264</v>
       </c>
-      <c r="G30" s="16"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I30" s="16"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="18">
         <v>30</v>
       </c>
@@ -4811,7 +5373,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="18">
         <v>31</v>
       </c>
@@ -5100,7 +5662,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="18">
         <v>48</v>
       </c>
@@ -5117,7 +5679,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="18">
         <v>49</v>
       </c>
@@ -5134,7 +5696,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="18">
         <v>50</v>
       </c>
@@ -5151,7 +5713,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="18">
         <v>51</v>
       </c>
@@ -5167,17 +5729,17 @@
       <c r="E52" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G52" s="22" t="s">
+      <c r="I52" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="H52" s="22" t="s">
+      <c r="J52" s="22" t="s">
         <v>201</v>
       </c>
-      <c r="I52" s="24" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K52" s="20" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="18">
         <v>52</v>
       </c>
@@ -5193,17 +5755,17 @@
       <c r="E53" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G53" s="23" t="s">
+      <c r="I53" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="H53" s="23" t="s">
+      <c r="J53" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="I53" s="25" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K53" s="19" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="18">
         <v>53</v>
       </c>
@@ -5219,17 +5781,17 @@
       <c r="E54" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G54" s="22" t="s">
+      <c r="I54" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="H54" s="22" t="s">
+      <c r="J54" s="22" t="s">
         <v>208</v>
       </c>
-      <c r="I54" s="24" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K54" s="20" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="18">
         <v>54</v>
       </c>
@@ -5245,17 +5807,17 @@
       <c r="E55" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G55" s="23" t="s">
+      <c r="I55" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="H55" s="23" t="s">
+      <c r="J55" s="23" t="s">
         <v>212</v>
       </c>
-      <c r="I55" s="25" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K55" s="19" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="18">
         <v>55</v>
       </c>
@@ -5271,17 +5833,17 @@
       <c r="E56" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G56" s="22" t="s">
+      <c r="I56" s="22" t="s">
         <v>227</v>
       </c>
-      <c r="H56" s="22" t="s">
+      <c r="J56" s="22" t="s">
         <v>228</v>
       </c>
-      <c r="I56" s="24" t="s">
+      <c r="K56" s="20" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="18">
         <v>56</v>
       </c>
@@ -5298,7 +5860,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="18">
         <v>57</v>
       </c>
@@ -5315,7 +5877,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="18">
         <v>58</v>
       </c>
@@ -5331,8 +5893,11 @@
       <c r="E59" s="16" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I59" s="19" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="18">
         <v>59</v>
       </c>
@@ -5348,8 +5913,11 @@
       <c r="E60" s="16" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I60" s="20" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="18">
         <v>60</v>
       </c>
@@ -5365,8 +5933,11 @@
       <c r="E61" s="16" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I61" s="19" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="18">
         <v>61</v>
       </c>
@@ -5382,8 +5953,11 @@
       <c r="E62" s="16" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I62" s="20" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="18">
         <v>62</v>
       </c>
@@ -5399,8 +5973,11 @@
       <c r="E63" s="16" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I63" s="19" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="18">
         <v>63</v>
       </c>
@@ -5417,7 +5994,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="18">
         <v>64</v>
       </c>
@@ -5433,8 +6010,11 @@
       <c r="E65" s="16" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I65" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="18">
         <v>65</v>
       </c>
@@ -5450,8 +6030,11 @@
       <c r="E66" s="16" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I66" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="18">
         <v>66</v>
       </c>
@@ -5467,8 +6050,11 @@
       <c r="E67" s="16" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I67" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="18">
         <v>67</v>
       </c>
@@ -5484,8 +6070,11 @@
       <c r="E68" s="16" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I68" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="18">
         <v>68</v>
       </c>
@@ -5501,8 +6090,11 @@
       <c r="E69" s="16" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I69" s="20" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="18">
         <v>69</v>
       </c>
@@ -5518,8 +6110,11 @@
       <c r="E70" s="16" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I70" s="19" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="18">
         <v>70</v>
       </c>
@@ -5535,8 +6130,11 @@
       <c r="E71" s="16" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I71" s="20" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="18">
         <v>71</v>
       </c>
@@ -5552,11 +6150,11 @@
       <c r="E72" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G72" s="19" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I72" s="19" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="18">
         <v>72</v>
       </c>
@@ -5572,11 +6170,8 @@
       <c r="E73" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="G73" s="20" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="18">
         <v>73</v>
       </c>
@@ -5592,11 +6187,17 @@
       <c r="E74" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="G74" s="19" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I74" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="J74" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="K74" s="25" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="18">
         <v>74</v>
       </c>
@@ -5613,11 +6214,19 @@
         <v>273</v>
       </c>
       <c r="F75" s="2"/>
-      <c r="G75" s="20" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
+      <c r="I75" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="J75" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="K75" s="27" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="18">
         <v>75</v>
       </c>
@@ -5634,11 +6243,19 @@
         <v>195</v>
       </c>
       <c r="F76" s="2"/>
-      <c r="G76" s="19" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="J76" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="K76" s="25" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="18">
         <v>76</v>
       </c>
@@ -5655,8 +6272,19 @@
         <v>195</v>
       </c>
       <c r="F77" s="2"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+      <c r="I77" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="J77" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="K77" s="27" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="18">
         <v>77</v>
       </c>
@@ -5672,11 +6300,17 @@
       <c r="E78" t="s">
         <v>260</v>
       </c>
-      <c r="G78" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I78" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="J78" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="K78" s="27" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="18">
         <v>78</v>
       </c>
@@ -5692,11 +6326,15 @@
       <c r="E79" t="s">
         <v>260</v>
       </c>
-      <c r="G79" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I79" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="J79" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="K79" s="25"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="18">
         <v>79</v>
       </c>
@@ -5712,11 +6350,17 @@
       <c r="E80" t="s">
         <v>260</v>
       </c>
-      <c r="G80" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I80" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="J80" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="K80" s="27" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="18">
         <v>80</v>
       </c>
@@ -5732,11 +6376,17 @@
       <c r="E81" t="s">
         <v>267</v>
       </c>
-      <c r="G81" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I81" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="J81" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="K81" s="25" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="18">
         <v>81</v>
       </c>
@@ -5752,11 +6402,8 @@
       <c r="E82" t="s">
         <v>195</v>
       </c>
-      <c r="G82" s="20" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="18">
         <v>82</v>
       </c>
@@ -5772,11 +6419,8 @@
       <c r="E83" t="s">
         <v>195</v>
       </c>
-      <c r="G83" s="19" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="18">
         <v>83</v>
       </c>
@@ -5792,11 +6436,8 @@
       <c r="E84" t="s">
         <v>195</v>
       </c>
-      <c r="G84" s="20" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="18">
         <v>84</v>
       </c>
@@ -5812,214 +6453,593 @@
       <c r="E85" t="s">
         <v>195</v>
       </c>
-      <c r="G85" s="19" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A86" s="18">
-        <v>85</v>
-      </c>
-      <c r="B86" s="18" t="s">
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A86" s="18"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="16"/>
+      <c r="D86" s="16"/>
+      <c r="E86" s="2"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A87" s="18"/>
+      <c r="B87" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C87" s="16"/>
+      <c r="D87" s="16"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A88" s="18"/>
+      <c r="C88" s="16"/>
+      <c r="D88" s="16"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A89" s="18"/>
+      <c r="B89" s="18"/>
+      <c r="C89" s="16"/>
+      <c r="D89" s="16"/>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A90" s="35" t="s">
+        <v>295</v>
+      </c>
+      <c r="B90" s="35" t="s">
+        <v>200</v>
+      </c>
+      <c r="C90" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="D90" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="E90" s="35" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A91" s="31" t="s">
+        <v>383</v>
+      </c>
+      <c r="B91" s="29" t="s">
         <v>372</v>
       </c>
-      <c r="C86" s="16" t="s">
+      <c r="C91" s="30" t="s">
         <v>323</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D91" s="32" t="s">
         <v>282</v>
       </c>
-      <c r="E86" s="16" t="s">
-        <v>260</v>
-      </c>
-      <c r="F86" s="2"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A87" s="18">
-        <v>86</v>
-      </c>
-      <c r="B87" s="18" t="s">
+      <c r="E91" s="30" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A92" s="31">
+        <v>2</v>
+      </c>
+      <c r="B92" s="31" t="s">
         <v>371</v>
       </c>
-      <c r="C87" s="16" t="s">
+      <c r="C92" s="32" t="s">
         <v>323</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D92" s="33" t="s">
         <v>283</v>
       </c>
-      <c r="E87" s="16" t="s">
-        <v>260</v>
-      </c>
-      <c r="F87" s="2"/>
-      <c r="G87" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="H87" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="I87" s="27" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A88" s="18">
-        <v>87</v>
-      </c>
-      <c r="B88" s="18" t="s">
+      <c r="E92" s="32" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A93" s="31">
+        <v>3</v>
+      </c>
+      <c r="B93" s="31" t="s">
         <v>373</v>
       </c>
-      <c r="C88" s="26" t="s">
+      <c r="C93" s="32" t="s">
         <v>323</v>
       </c>
-      <c r="D88" s="26" t="s">
+      <c r="D93" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="E88" s="27" t="s">
-        <v>260</v>
-      </c>
-      <c r="F88" s="2"/>
-      <c r="G88" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="H88" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="I88" s="29" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A89" s="18">
-        <v>88</v>
-      </c>
-      <c r="B89" s="2" t="s">
+      <c r="E93" s="32" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A94" s="31">
+        <v>4</v>
+      </c>
+      <c r="B94" s="34" t="s">
         <v>374</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C94" s="33" t="s">
         <v>323</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D94" s="33" t="s">
         <v>281</v>
       </c>
-      <c r="E89" t="s">
-        <v>260</v>
-      </c>
-      <c r="F89" s="2"/>
-      <c r="G89" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="H89" s="26" t="s">
-        <v>168</v>
-      </c>
-      <c r="I89" s="27" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A90" s="18">
-        <v>89</v>
-      </c>
-      <c r="B90" s="2" t="s">
+      <c r="E94" s="33" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A95" s="31">
+        <v>5</v>
+      </c>
+      <c r="B95" s="34" t="s">
         <v>370</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C95" s="33" t="s">
         <v>322</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D95" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="E90" t="s">
-        <v>260</v>
-      </c>
-      <c r="F90" s="2"/>
-      <c r="G90" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="H90" s="28" t="s">
-        <v>176</v>
-      </c>
-      <c r="I90" s="29" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A91" s="18">
-        <v>90</v>
-      </c>
-      <c r="B91" s="2" t="s">
+      <c r="E95" s="33" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A96" s="31">
+        <v>6</v>
+      </c>
+      <c r="B96" s="34" t="s">
         <v>375</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C96" s="33" t="s">
         <v>322</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D96" s="33" t="s">
         <v>199</v>
       </c>
-      <c r="E91" t="s">
+      <c r="E96" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="F91" s="2"/>
-      <c r="G91" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="H91" s="28" t="s">
-        <v>160</v>
-      </c>
-      <c r="I91" s="29" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A92" s="18"/>
-      <c r="B92" s="2"/>
-      <c r="C92" s="16"/>
-      <c r="D92" s="16"/>
-      <c r="E92" s="2"/>
-      <c r="G92" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="H92" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="I92" s="27"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A93" s="18"/>
-      <c r="B93" s="2"/>
-      <c r="C93" s="16"/>
-      <c r="D93" s="16"/>
-      <c r="G93" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="H93" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="I93" s="29" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A94" s="18"/>
-      <c r="B94" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="C94" s="16"/>
-      <c r="D94" s="16"/>
-      <c r="G94" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="H94" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="I94" s="27" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A95" s="18"/>
-      <c r="B95" s="18"/>
-      <c r="C95" s="16"/>
-      <c r="D95" s="16"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" s="35" t="s">
+        <v>295</v>
+      </c>
+      <c r="B100" s="35" t="s">
+        <v>200</v>
+      </c>
+      <c r="C100" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="D100" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="E100" s="35" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" s="36">
+        <v>1</v>
+      </c>
+      <c r="B101" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="C101" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="D101" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="E101" s="26" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" s="37">
+        <v>2</v>
+      </c>
+      <c r="B102" s="37" t="s">
+        <v>286</v>
+      </c>
+      <c r="C102" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="D102" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="E102" s="24" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" s="36">
+        <v>3</v>
+      </c>
+      <c r="B103" s="36" t="s">
+        <v>287</v>
+      </c>
+      <c r="C103" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="D103" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="E103" s="26" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" s="37">
+        <v>4</v>
+      </c>
+      <c r="B104" s="37" t="s">
+        <v>288</v>
+      </c>
+      <c r="C104" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="D104" s="24" t="s">
+        <v>262</v>
+      </c>
+      <c r="E104" s="24" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" s="36">
+        <v>5</v>
+      </c>
+      <c r="B105" s="36" t="s">
+        <v>289</v>
+      </c>
+      <c r="C105" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="D105" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="E105" s="26" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" s="37">
+        <v>6</v>
+      </c>
+      <c r="B106" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="C106" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="D106" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="E106" s="24" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" s="36">
+        <v>7</v>
+      </c>
+      <c r="B107" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="C107" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="D107" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="E107" s="26" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" s="37">
+        <v>8</v>
+      </c>
+      <c r="B108" s="37" t="s">
+        <v>299</v>
+      </c>
+      <c r="C108" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="D108" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="E108" s="24" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" s="36">
+        <v>9</v>
+      </c>
+      <c r="B109" s="36" t="s">
+        <v>300</v>
+      </c>
+      <c r="C109" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="D109" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="E109" s="26" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" s="37">
+        <v>10</v>
+      </c>
+      <c r="B110" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="C110" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="D110" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="E110" s="24" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" s="36">
+        <v>11</v>
+      </c>
+      <c r="B111" s="36" t="s">
+        <v>302</v>
+      </c>
+      <c r="C111" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="D111" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="E111" s="26" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" s="37">
+        <v>12</v>
+      </c>
+      <c r="B112" s="37" t="s">
+        <v>308</v>
+      </c>
+      <c r="C112" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="D112" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="E112" s="24" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" s="36">
+        <v>13</v>
+      </c>
+      <c r="B113" s="36" t="s">
+        <v>310</v>
+      </c>
+      <c r="C113" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="D113" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="E113" s="26" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" s="37">
+        <v>14</v>
+      </c>
+      <c r="B114" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="C114" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="D114" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="E114" s="24" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" s="36">
+        <v>15</v>
+      </c>
+      <c r="B115" s="38" t="s">
+        <v>324</v>
+      </c>
+      <c r="C115" s="22" t="s">
+        <v>323</v>
+      </c>
+      <c r="D115" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="E115" s="26" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116" s="37">
+        <v>16</v>
+      </c>
+      <c r="B116" s="39" t="s">
+        <v>326</v>
+      </c>
+      <c r="C116" s="23" t="s">
+        <v>323</v>
+      </c>
+      <c r="D116" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="E116" s="24" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117" s="36">
+        <v>17</v>
+      </c>
+      <c r="B117" s="38" t="s">
+        <v>331</v>
+      </c>
+      <c r="C117" s="22" t="s">
+        <v>323</v>
+      </c>
+      <c r="D117" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="E117" s="26" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118" s="37">
+        <v>18</v>
+      </c>
+      <c r="B118" s="39" t="s">
+        <v>336</v>
+      </c>
+      <c r="C118" s="23" t="s">
+        <v>323</v>
+      </c>
+      <c r="D118" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="E118" s="24" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119" s="36">
+        <v>19</v>
+      </c>
+      <c r="B119" s="36" t="s">
+        <v>351</v>
+      </c>
+      <c r="C119" s="26" t="s">
+        <v>379</v>
+      </c>
+      <c r="D119" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="E119" s="26" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120" s="37">
+        <v>20</v>
+      </c>
+      <c r="B120" s="37" t="s">
+        <v>372</v>
+      </c>
+      <c r="C120" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="D120" s="24" t="s">
+        <v>282</v>
+      </c>
+      <c r="E120" s="24" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121" s="36">
+        <v>21</v>
+      </c>
+      <c r="B121" s="38" t="s">
+        <v>371</v>
+      </c>
+      <c r="C121" s="22" t="s">
+        <v>323</v>
+      </c>
+      <c r="D121" s="22" t="s">
+        <v>283</v>
+      </c>
+      <c r="E121" s="26" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122" s="37">
+        <v>22</v>
+      </c>
+      <c r="B122" s="39" t="s">
+        <v>373</v>
+      </c>
+      <c r="C122" s="23" t="s">
+        <v>323</v>
+      </c>
+      <c r="D122" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="E122" s="24" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123" s="36">
+        <v>23</v>
+      </c>
+      <c r="B123" s="38" t="s">
+        <v>374</v>
+      </c>
+      <c r="C123" s="22" t="s">
+        <v>323</v>
+      </c>
+      <c r="D123" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="E123" s="26" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124" s="37">
+        <v>23</v>
+      </c>
+      <c r="B124" s="39" t="s">
+        <v>370</v>
+      </c>
+      <c r="C124" s="23" t="s">
+        <v>322</v>
+      </c>
+      <c r="D124" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="E124" s="24" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125" s="31">
+        <v>25</v>
+      </c>
+      <c r="B125" s="40" t="s">
+        <v>375</v>
+      </c>
+      <c r="C125" s="33" t="s">
+        <v>322</v>
+      </c>
+      <c r="D125" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="E125" s="32" t="s">
+        <v>195</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -6029,24 +7049,31 @@
     <hyperlink ref="D79" r:id="rId4" display="https://www.sciencedirect.com/science/article/pii/S0740624X11000700" xr:uid="{824828A2-F964-8B4D-83D3-6EDCEC70C76D}"/>
     <hyperlink ref="D80" r:id="rId5" display="https://www.sciencedirect.com/science/article/pii/S2472630322015850" xr:uid="{6490D629-B338-4A44-AE9D-93E8362F01DA}"/>
     <hyperlink ref="D81" r:id="rId6" display="https://www.sciencedirect.com/science/article/pii/S2212017313002892" xr:uid="{475DCFD4-127F-F042-93CF-BA4A7561A4FF}"/>
-    <hyperlink ref="D91" r:id="rId7" display="https://research.tue.nl/files/3123158/200910510.pdf" xr:uid="{F41A079D-1CF9-6C4D-A340-2DF19553BC1C}"/>
-    <hyperlink ref="D2" r:id="rId8" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000499808400012" xr:uid="{12545708-E73D-8F4A-AFEE-1269B5901374}"/>
-    <hyperlink ref="D6" r:id="rId9" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000886542700027" xr:uid="{58F3C534-2B26-204D-AA9D-745EB54218D5}"/>
-    <hyperlink ref="D8" r:id="rId10" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000362796900054" xr:uid="{0526D87E-6A63-BC42-AC45-963B4F480177}"/>
-    <hyperlink ref="D20" r:id="rId11" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000441748200002" xr:uid="{3EC13A01-81F6-6040-A0C3-28F4BE54096B}"/>
-    <hyperlink ref="D30" r:id="rId12" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000657137400001" xr:uid="{28DFAF60-E1CD-944B-A6CA-B463BB8D10CA}"/>
-    <hyperlink ref="D29" r:id="rId13" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000412130500026" xr:uid="{054ECBD1-B80D-9441-9905-D3CBDBCCCA3F}"/>
-    <hyperlink ref="D28" r:id="rId14" display="https://www.webofscience.com/wos/woscc/full-record/WOS:001028026200001" xr:uid="{F2465AB0-E763-774E-9DC6-B83E270148CF}"/>
-    <hyperlink ref="D27" r:id="rId15" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000369170600012" xr:uid="{93E32600-8C35-D743-8574-D9C506553033}"/>
-    <hyperlink ref="D25" r:id="rId16" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000510227000019" xr:uid="{279A67FC-0599-0B4F-A7C7-B3303F055683}"/>
-    <hyperlink ref="D26" r:id="rId17" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000919783700001" xr:uid="{CBA6F9A3-CDD0-BF48-A937-93DA1BCDFBDD}"/>
-    <hyperlink ref="D22" r:id="rId18" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000789418000027" xr:uid="{682DF916-DD6D-B149-8715-BFD26D22CD2A}"/>
-    <hyperlink ref="D23" r:id="rId19" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000383949300135" xr:uid="{ADB1B83E-1F66-1A4E-BDB6-26AF05AA9C32}"/>
-    <hyperlink ref="D24" r:id="rId20" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000432839500046" xr:uid="{6F302675-F45F-5C44-87DF-681D368209AA}"/>
+    <hyperlink ref="D2" r:id="rId7" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000499808400012" xr:uid="{12545708-E73D-8F4A-AFEE-1269B5901374}"/>
+    <hyperlink ref="D6" r:id="rId8" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000886542700027" xr:uid="{58F3C534-2B26-204D-AA9D-745EB54218D5}"/>
+    <hyperlink ref="D8" r:id="rId9" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000362796900054" xr:uid="{0526D87E-6A63-BC42-AC45-963B4F480177}"/>
+    <hyperlink ref="D20" r:id="rId10" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000441748200002" xr:uid="{3EC13A01-81F6-6040-A0C3-28F4BE54096B}"/>
+    <hyperlink ref="D30" r:id="rId11" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000657137400001" xr:uid="{28DFAF60-E1CD-944B-A6CA-B463BB8D10CA}"/>
+    <hyperlink ref="D29" r:id="rId12" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000412130500026" xr:uid="{054ECBD1-B80D-9441-9905-D3CBDBCCCA3F}"/>
+    <hyperlink ref="D28" r:id="rId13" display="https://www.webofscience.com/wos/woscc/full-record/WOS:001028026200001" xr:uid="{F2465AB0-E763-774E-9DC6-B83E270148CF}"/>
+    <hyperlink ref="D27" r:id="rId14" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000369170600012" xr:uid="{93E32600-8C35-D743-8574-D9C506553033}"/>
+    <hyperlink ref="D25" r:id="rId15" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000510227000019" xr:uid="{279A67FC-0599-0B4F-A7C7-B3303F055683}"/>
+    <hyperlink ref="D26" r:id="rId16" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000919783700001" xr:uid="{CBA6F9A3-CDD0-BF48-A937-93DA1BCDFBDD}"/>
+    <hyperlink ref="D22" r:id="rId17" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000789418000027" xr:uid="{682DF916-DD6D-B149-8715-BFD26D22CD2A}"/>
+    <hyperlink ref="D23" r:id="rId18" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000383949300135" xr:uid="{ADB1B83E-1F66-1A4E-BDB6-26AF05AA9C32}"/>
+    <hyperlink ref="D24" r:id="rId19" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000432839500046" xr:uid="{6F302675-F45F-5C44-87DF-681D368209AA}"/>
+    <hyperlink ref="D96" r:id="rId20" display="https://research.tue.nl/files/3123158/200910510.pdf" xr:uid="{2414FA0E-238B-1648-9B59-24BB65CDDC99}"/>
+    <hyperlink ref="D104" r:id="rId21" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000886542700027" xr:uid="{209C6EAE-1525-1649-A506-592C8B38042D}"/>
+    <hyperlink ref="D112" r:id="rId22" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000919783700001" xr:uid="{7CE7FC99-2C51-E047-990C-3FE670585B92}"/>
+    <hyperlink ref="D113" r:id="rId23" display="https://www.webofscience.com/wos/woscc/full-record/WOS:001028026200001" xr:uid="{B6123B0B-4E3B-7940-88DF-68F00A6FD32F}"/>
+    <hyperlink ref="D114" r:id="rId24" display="https://www.webofscience.com/wos/woscc/full-record/WOS:000657137400001" xr:uid="{F5CE7EB2-6920-DC40-97C1-7D03A6D98006}"/>
+    <hyperlink ref="D125" r:id="rId25" display="https://research.tue.nl/files/3123158/200910510.pdf" xr:uid="{BC477476-1AA0-6A4D-A908-31667AE823B1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId21"/>
+  <tableParts count="3">
+    <tablePart r:id="rId26"/>
+    <tablePart r:id="rId27"/>
+    <tablePart r:id="rId28"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
After adding global _variables
</commit_message>
<xml_diff>
--- a/tables/slr_logbook.xlsx
+++ b/tables/slr_logbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Projects/literature/phd_kul/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9DECB5-04CB-F845-9934-59B9F6197480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6202368-36C1-454B-A98E-1CACFFD6D2F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36120" yWindow="500" windowWidth="38120" windowHeight="41300" activeTab="1" xr2:uid="{AC0C9749-44FB-E246-A4D0-62D1F20133DE}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="385">
   <si>
     <t>Date</t>
   </si>
@@ -717,9 +717,6 @@
     <t>Comparative Analysis of Business Process Modelling Tools for Compliance Management Support</t>
   </si>
   <si>
-    <t>Embracing Process Compliance and Flexibility Through Behavioral Consistency Checking in {ACM} - {A} Repair Service Management Case</t>
-  </si>
-  <si>
     <t>Managing Regulatory Compliance in Business Processes</t>
   </si>
   <si>
@@ -775,9 +772,6 @@
   </si>
   <si>
     <t>A compliance management framework for business process models</t>
-  </si>
-  <si>
-    <t>Business Control Management - {A} Discipline to Ensure Regulatory Compliance of {SOA} Applications</t>
   </si>
   <si>
     <t>Business Process Compliance Tracking Using Key Performance Indicators</t>
@@ -1261,6 +1255,15 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>Embracing Process Compliance and Flexibility Through Behavioral Consistency Checking in ACM - A Repair Service Management Case</t>
+  </si>
+  <si>
+    <t>Business Control Management - A Discipline to Ensure Regulatory Compliance of {SOA} Applications</t>
+  </si>
+  <si>
+    <t>Business Process Modelling in Healthcare and Compliance Management: A Logical Framework</t>
   </si>
 </sst>
 </file>
@@ -4699,7 +4702,7 @@
   <dimension ref="A1:K125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100:E125"/>
+      <selection activeCell="E118" sqref="E118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4715,7 +4718,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>200</v>
@@ -4727,10 +4730,10 @@
         <v>178</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J1" s="16"/>
     </row>
@@ -4739,16 +4742,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I2" s="16"/>
     </row>
@@ -4757,16 +4760,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>179</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
@@ -4776,16 +4779,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>181</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I4" s="16"/>
       <c r="J4" s="16"/>
@@ -4795,16 +4798,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>189</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I5" s="26" t="s">
         <v>157</v>
@@ -4813,7 +4816,7 @@
         <v>175</v>
       </c>
       <c r="K5" s="27" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -4821,16 +4824,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I6" s="24" t="s">
         <v>157</v>
@@ -4839,7 +4842,7 @@
         <v>170</v>
       </c>
       <c r="K6" s="25" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -4847,16 +4850,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>166</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I7" s="26" t="s">
         <v>157</v>
@@ -4865,7 +4868,7 @@
         <v>169</v>
       </c>
       <c r="K7" s="27" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -4873,16 +4876,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I8" s="24" t="s">
         <v>157</v>
@@ -4891,7 +4894,7 @@
         <v>163</v>
       </c>
       <c r="K8" s="25" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -4899,16 +4902,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>190</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I9" s="28" t="s">
         <v>157</v>
@@ -4917,7 +4920,7 @@
         <v>158</v>
       </c>
       <c r="K9" s="27" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -4925,16 +4928,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>191</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I10" s="24" t="s">
         <v>157</v>
@@ -4943,7 +4946,7 @@
         <v>161</v>
       </c>
       <c r="K10" s="25" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -4951,16 +4954,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>192</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I11" s="26" t="s">
         <v>157</v>
@@ -4969,7 +4972,7 @@
         <v>165</v>
       </c>
       <c r="K11" s="27" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -4977,16 +4980,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>193</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I12" s="24" t="s">
         <v>157</v>
@@ -4995,7 +4998,7 @@
         <v>188</v>
       </c>
       <c r="K12" s="25" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -5003,16 +5006,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D13" s="16" t="s">
         <v>194</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I13" s="26" t="s">
         <v>157</v>
@@ -5021,7 +5024,7 @@
         <v>196</v>
       </c>
       <c r="K13" s="27" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -5029,16 +5032,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D14" s="16" t="s">
         <v>180</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I14" s="24" t="s">
         <v>157</v>
@@ -5047,7 +5050,7 @@
         <v>180</v>
       </c>
       <c r="K14" s="25" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -5055,16 +5058,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D15" s="16" t="s">
         <v>182</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I15" s="26" t="s">
         <v>157</v>
@@ -5073,7 +5076,7 @@
         <v>167</v>
       </c>
       <c r="K15" s="27" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -5081,16 +5084,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>183</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I16" s="24" t="s">
         <v>157</v>
@@ -5099,7 +5102,7 @@
         <v>197</v>
       </c>
       <c r="K16" s="25" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -5107,16 +5110,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>184</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I17" s="16"/>
     </row>
@@ -5125,16 +5128,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>185</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I18" s="16"/>
     </row>
@@ -5143,16 +5146,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D19" s="16" t="s">
         <v>186</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I19" s="16"/>
     </row>
@@ -5161,16 +5164,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D20" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="E20" s="16" t="s">
         <v>265</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>267</v>
       </c>
       <c r="I20" s="16"/>
     </row>
@@ -5179,16 +5182,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D21" s="16" t="s">
         <v>187</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I21" s="16"/>
     </row>
@@ -5197,16 +5200,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I22" s="16"/>
     </row>
@@ -5215,16 +5218,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I23" s="16"/>
     </row>
@@ -5233,16 +5236,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I24" s="16"/>
     </row>
@@ -5251,16 +5254,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I25" s="16"/>
     </row>
@@ -5269,19 +5272,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I26" s="16" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -5289,16 +5292,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I27" s="16"/>
     </row>
@@ -5307,16 +5310,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I28" s="16"/>
     </row>
@@ -5325,16 +5328,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I29" s="16"/>
     </row>
@@ -5343,16 +5346,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I30" s="16"/>
     </row>
@@ -5361,16 +5364,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C31" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D31" t="s">
         <v>201</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -5378,16 +5381,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C32" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D32" t="s">
         <v>202</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -5395,16 +5398,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C33" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D33" t="s">
         <v>203</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -5412,16 +5415,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C34" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D34" t="s">
         <v>204</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -5429,16 +5432,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C35" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D35" t="s">
         <v>205</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -5446,16 +5449,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C36" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D36" t="s">
         <v>206</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -5463,16 +5466,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C37" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D37" t="s">
         <v>207</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -5480,16 +5483,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C38" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D38" t="s">
         <v>208</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -5497,16 +5500,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C39" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D39" t="s">
-        <v>209</v>
+        <v>382</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -5514,16 +5517,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C40" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D40" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -5531,16 +5534,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C41" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D41" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -5548,13 +5551,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C42" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D42" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E42" s="16" t="s">
         <v>195</v>
@@ -5565,16 +5568,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C43" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D43" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -5582,16 +5585,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C44" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D44" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -5599,16 +5602,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C45" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D45" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -5616,16 +5619,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C46" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D46" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -5633,16 +5636,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C47" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D47" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -5650,16 +5653,16 @@
         <v>47</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C48" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D48" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
@@ -5667,16 +5670,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C49" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D49" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E49" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
@@ -5684,16 +5687,16 @@
         <v>49</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C50" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D50" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E50" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
@@ -5701,16 +5704,16 @@
         <v>50</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C51" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D51" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
@@ -5718,16 +5721,16 @@
         <v>51</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C52" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D52" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I52" s="22" t="s">
         <v>159</v>
@@ -5736,7 +5739,7 @@
         <v>201</v>
       </c>
       <c r="K52" s="20" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
@@ -5744,16 +5747,16 @@
         <v>52</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C53" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D53" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E53" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I53" s="23" t="s">
         <v>159</v>
@@ -5762,7 +5765,7 @@
         <v>203</v>
       </c>
       <c r="K53" s="19" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -5770,16 +5773,16 @@
         <v>53</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C54" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D54" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I54" s="22" t="s">
         <v>159</v>
@@ -5788,7 +5791,7 @@
         <v>208</v>
       </c>
       <c r="K54" s="20" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -5796,25 +5799,25 @@
         <v>54</v>
       </c>
       <c r="B55" s="21" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C55" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D55" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E55" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I55" s="23" t="s">
         <v>159</v>
       </c>
       <c r="J55" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K55" s="19" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -5822,22 +5825,22 @@
         <v>55</v>
       </c>
       <c r="B56" s="21" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C56" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D56" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I56" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="J56" s="22" t="s">
         <v>227</v>
-      </c>
-      <c r="J56" s="22" t="s">
-        <v>228</v>
       </c>
       <c r="K56" s="20" t="s">
         <v>195</v>
@@ -5848,16 +5851,16 @@
         <v>56</v>
       </c>
       <c r="B57" s="21" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C57" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D57" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E57" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
@@ -5865,16 +5868,16 @@
         <v>57</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C58" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D58" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E58" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -5882,19 +5885,19 @@
         <v>58</v>
       </c>
       <c r="B59" s="21" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C59" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D59" t="s">
-        <v>229</v>
+        <v>383</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I59" s="19" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -5902,19 +5905,19 @@
         <v>59</v>
       </c>
       <c r="B60" s="21" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C60" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D60" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I60" s="20" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -5922,19 +5925,19 @@
         <v>60</v>
       </c>
       <c r="B61" s="21" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C61" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D61" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I61" s="19" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -5942,19 +5945,19 @@
         <v>61</v>
       </c>
       <c r="B62" s="21" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C62" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D62" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I62" s="20" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
@@ -5962,19 +5965,19 @@
         <v>62</v>
       </c>
       <c r="B63" s="21" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C63" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D63" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E63" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I63" s="19" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
@@ -5982,16 +5985,16 @@
         <v>63</v>
       </c>
       <c r="B64" s="21" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C64" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D64" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E64" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
@@ -5999,16 +6002,16 @@
         <v>64</v>
       </c>
       <c r="B65" s="21" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C65" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D65" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E65" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I65" s="2" t="s">
         <v>195</v>
@@ -6019,16 +6022,16 @@
         <v>65</v>
       </c>
       <c r="B66" s="21" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C66" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D66" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E66" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>195</v>
@@ -6039,16 +6042,16 @@
         <v>66</v>
       </c>
       <c r="B67" s="21" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C67" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D67" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E67" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I67" s="2" t="s">
         <v>195</v>
@@ -6059,16 +6062,16 @@
         <v>67</v>
       </c>
       <c r="B68" s="21" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C68" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D68" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E68" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I68" s="2" t="s">
         <v>195</v>
@@ -6079,19 +6082,19 @@
         <v>68</v>
       </c>
       <c r="B69" s="21" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C69" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D69" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E69" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I69" s="20" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
@@ -6099,19 +6102,19 @@
         <v>69</v>
       </c>
       <c r="B70" s="21" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C70" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D70" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E70" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I70" s="19" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
@@ -6119,19 +6122,19 @@
         <v>70</v>
       </c>
       <c r="B71" s="21" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C71" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D71" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E71" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I71" s="20" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
@@ -6139,19 +6142,19 @@
         <v>71</v>
       </c>
       <c r="B72" s="21" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C72" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D72" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E72" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I72" s="19" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
@@ -6159,16 +6162,16 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C73" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D73" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E73" s="16" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
@@ -6176,13 +6179,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C74" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D74" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E74" s="16" t="s">
         <v>195</v>
@@ -6194,7 +6197,7 @@
         <v>172</v>
       </c>
       <c r="K74" s="25" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
@@ -6202,16 +6205,16 @@
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C75" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D75" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E75" s="16" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
@@ -6223,7 +6226,7 @@
         <v>171</v>
       </c>
       <c r="K75" s="27" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
@@ -6231,13 +6234,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C76" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D76" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E76" s="16" t="s">
         <v>195</v>
@@ -6252,7 +6255,7 @@
         <v>168</v>
       </c>
       <c r="K76" s="25" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
@@ -6260,13 +6263,13 @@
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C77" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D77" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E77" s="16" t="s">
         <v>195</v>
@@ -6281,7 +6284,7 @@
         <v>176</v>
       </c>
       <c r="K77" s="27" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
@@ -6289,16 +6292,16 @@
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C78" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D78" t="s">
         <v>192</v>
       </c>
       <c r="E78" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I78" s="26" t="s">
         <v>159</v>
@@ -6307,7 +6310,7 @@
         <v>160</v>
       </c>
       <c r="K78" s="27" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
@@ -6315,16 +6318,16 @@
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C79" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D79" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E79" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I79" s="24" t="s">
         <v>159</v>
@@ -6339,16 +6342,16 @@
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C80" t="s">
         <v>320</v>
-      </c>
-      <c r="C80" t="s">
-        <v>322</v>
       </c>
       <c r="D80" t="s">
         <v>185</v>
       </c>
       <c r="E80" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I80" s="26" t="s">
         <v>159</v>
@@ -6357,7 +6360,7 @@
         <v>162</v>
       </c>
       <c r="K80" s="27" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
@@ -6365,16 +6368,16 @@
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C81" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D81" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E81" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I81" s="24" t="s">
         <v>159</v>
@@ -6383,7 +6386,7 @@
         <v>164</v>
       </c>
       <c r="K81" s="25" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
@@ -6391,13 +6394,13 @@
         <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C82" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D82" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E82" t="s">
         <v>195</v>
@@ -6408,13 +6411,13 @@
         <v>82</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C83" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D83" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E83" t="s">
         <v>195</v>
@@ -6425,13 +6428,13 @@
         <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C84" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D84" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E84" t="s">
         <v>195</v>
@@ -6442,13 +6445,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C85" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D85" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E85" t="s">
         <v>195</v>
@@ -6464,7 +6467,7 @@
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="18"/>
       <c r="B87" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C87" s="16"/>
       <c r="D87" s="16"/>
@@ -6482,7 +6485,7 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="35" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B90" s="35" t="s">
         <v>200</v>
@@ -6494,24 +6497,24 @@
         <v>178</v>
       </c>
       <c r="E90" s="35" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="31" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B91" s="29" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C91" s="30" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D91" s="32" t="s">
-        <v>282</v>
-      </c>
-      <c r="E91" s="30" t="s">
-        <v>260</v>
+        <v>280</v>
+      </c>
+      <c r="E91" s="32" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
@@ -6519,16 +6522,16 @@
         <v>2</v>
       </c>
       <c r="B92" s="31" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C92" s="32" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D92" s="33" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E92" s="32" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
@@ -6536,16 +6539,16 @@
         <v>3</v>
       </c>
       <c r="B93" s="31" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C93" s="32" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D93" s="32" t="s">
         <v>173</v>
       </c>
       <c r="E93" s="32" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
@@ -6553,16 +6556,16 @@
         <v>4</v>
       </c>
       <c r="B94" s="34" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C94" s="33" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D94" s="33" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E94" s="33" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
@@ -6570,16 +6573,16 @@
         <v>5</v>
       </c>
       <c r="B95" s="34" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C95" s="33" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D95" s="33" t="s">
         <v>198</v>
       </c>
       <c r="E95" s="33" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
@@ -6587,21 +6590,21 @@
         <v>6</v>
       </c>
       <c r="B96" s="34" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C96" s="33" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D96" s="33" t="s">
         <v>199</v>
       </c>
-      <c r="E96" s="33" t="s">
-        <v>195</v>
+      <c r="E96" s="32" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="35" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B100" s="35" t="s">
         <v>200</v>
@@ -6613,7 +6616,7 @@
         <v>178</v>
       </c>
       <c r="E100" s="35" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -6621,16 +6624,16 @@
         <v>1</v>
       </c>
       <c r="B101" s="36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C101" s="26" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D101" s="26" t="s">
         <v>179</v>
       </c>
       <c r="E101" s="26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
@@ -6638,16 +6641,16 @@
         <v>2</v>
       </c>
       <c r="B102" s="37" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C102" s="24" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D102" s="24" t="s">
         <v>181</v>
       </c>
       <c r="E102" s="24" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -6655,16 +6658,16 @@
         <v>3</v>
       </c>
       <c r="B103" s="36" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C103" s="26" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D103" s="26" t="s">
         <v>189</v>
       </c>
       <c r="E103" s="26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -6672,16 +6675,16 @@
         <v>4</v>
       </c>
       <c r="B104" s="37" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C104" s="24" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D104" s="24" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E104" s="24" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -6689,16 +6692,16 @@
         <v>5</v>
       </c>
       <c r="B105" s="36" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C105" s="26" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D105" s="26" t="s">
         <v>166</v>
       </c>
       <c r="E105" s="26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -6706,16 +6709,16 @@
         <v>6</v>
       </c>
       <c r="B106" s="37" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C106" s="24" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D106" s="24" t="s">
         <v>192</v>
       </c>
       <c r="E106" s="24" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
@@ -6723,16 +6726,16 @@
         <v>7</v>
       </c>
       <c r="B107" s="36" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C107" s="26" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D107" s="26" t="s">
         <v>182</v>
       </c>
       <c r="E107" s="26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -6740,16 +6743,16 @@
         <v>8</v>
       </c>
       <c r="B108" s="37" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C108" s="24" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D108" s="24" t="s">
         <v>183</v>
       </c>
       <c r="E108" s="24" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -6757,16 +6760,16 @@
         <v>9</v>
       </c>
       <c r="B109" s="36" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C109" s="26" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D109" s="26" t="s">
         <v>184</v>
       </c>
       <c r="E109" s="26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -6774,16 +6777,16 @@
         <v>10</v>
       </c>
       <c r="B110" s="37" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C110" s="24" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D110" s="24" t="s">
         <v>185</v>
       </c>
       <c r="E110" s="24" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -6791,16 +6794,16 @@
         <v>11</v>
       </c>
       <c r="B111" s="36" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C111" s="26" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D111" s="26" t="s">
         <v>186</v>
       </c>
       <c r="E111" s="26" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -6808,16 +6811,16 @@
         <v>12</v>
       </c>
       <c r="B112" s="37" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C112" s="24" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D112" s="24" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E112" s="24" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -6825,16 +6828,16 @@
         <v>13</v>
       </c>
       <c r="B113" s="36" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C113" s="26" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D113" s="26" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E113" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -6842,16 +6845,16 @@
         <v>14</v>
       </c>
       <c r="B114" s="37" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C114" s="24" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D114" s="24" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E114" s="24" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -6859,16 +6862,16 @@
         <v>15</v>
       </c>
       <c r="B115" s="38" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C115" s="22" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D115" s="22" t="s">
-        <v>201</v>
+        <v>384</v>
       </c>
       <c r="E115" s="26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -6876,16 +6879,16 @@
         <v>16</v>
       </c>
       <c r="B116" s="39" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C116" s="23" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D116" s="23" t="s">
         <v>203</v>
       </c>
       <c r="E116" s="24" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -6893,16 +6896,16 @@
         <v>17</v>
       </c>
       <c r="B117" s="38" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C117" s="22" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D117" s="22" t="s">
         <v>208</v>
       </c>
       <c r="E117" s="26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -6910,16 +6913,16 @@
         <v>18</v>
       </c>
       <c r="B118" s="39" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C118" s="23" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D118" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E118" s="24" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -6927,16 +6930,16 @@
         <v>19</v>
       </c>
       <c r="B119" s="36" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C119" s="26" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D119" s="26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E119" s="26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -6944,16 +6947,16 @@
         <v>20</v>
       </c>
       <c r="B120" s="37" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C120" s="24" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D120" s="24" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E120" s="24" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -6961,16 +6964,16 @@
         <v>21</v>
       </c>
       <c r="B121" s="38" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C121" s="22" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D121" s="22" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E121" s="26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
@@ -6978,16 +6981,16 @@
         <v>22</v>
       </c>
       <c r="B122" s="39" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C122" s="23" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D122" s="23" t="s">
         <v>173</v>
       </c>
       <c r="E122" s="24" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -6995,16 +6998,16 @@
         <v>23</v>
       </c>
       <c r="B123" s="38" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C123" s="22" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D123" s="22" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E123" s="26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
@@ -7012,16 +7015,16 @@
         <v>23</v>
       </c>
       <c r="B124" s="39" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C124" s="23" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D124" s="23" t="s">
         <v>198</v>
       </c>
       <c r="E124" s="24" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
@@ -7029,16 +7032,16 @@
         <v>25</v>
       </c>
       <c r="B125" s="40" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C125" s="33" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D125" s="33" t="s">
         <v>199</v>
       </c>
-      <c r="E125" s="32" t="s">
-        <v>195</v>
+      <c r="E125" s="26" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2024-04-10 Update Separated s1
</commit_message>
<xml_diff>
--- a/tables/slr_logbook.xlsx
+++ b/tables/slr_logbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Projects/literature/phd_kul/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3BC0879-249D-F54C-88A8-7FA3295DFDD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDDF7BD-96E9-AB4B-B866-F1269F8DD12F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27240" yWindow="500" windowWidth="43080" windowHeight="42700" activeTab="1" xr2:uid="{AC0C9749-44FB-E246-A4D0-62D1F20133DE}"/>
   </bookViews>
@@ -5566,7 +5566,7 @@
   <dimension ref="A1:AA130"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D123" sqref="D123"/>
+      <selection activeCell="A129" sqref="A129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8575,7 +8575,7 @@
     </row>
     <row r="122" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A122" s="25">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B122" s="39" t="s">
         <v>299</v>
@@ -8617,7 +8617,7 @@
     </row>
     <row r="124" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A124" s="26">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B124" s="40" t="s">
         <v>298</v>
@@ -8638,7 +8638,7 @@
     </row>
     <row r="125" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A125" s="25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B125" s="39" t="s">
         <v>223</v>
@@ -8659,7 +8659,7 @@
     </row>
     <row r="126" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A126" s="26">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B126" s="40" t="s">
         <v>250</v>
@@ -8680,7 +8680,7 @@
     </row>
     <row r="127" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A127" s="25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B127" s="39" t="s">
         <v>297</v>
@@ -8701,7 +8701,7 @@
     </row>
     <row r="128" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A128" s="25">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B128" s="39" t="s">
         <v>211</v>
@@ -8722,7 +8722,7 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" s="25">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B129" s="39" t="s">
         <v>217</v>
@@ -8743,7 +8743,7 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" s="58">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B130" s="59" t="s">
         <v>222</v>

</xml_diff>